<commit_message>
Cleared up response types
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -11303,7 +11303,7 @@
     <t>Detect</t>
   </si>
   <si>
-    <t>discover or discern the existence, presence, or fact of an intrusion into information systems. We included Detect because that’s what everyone was doing - looking, not reacting, and we wanted them to get that out of their systems.</t>
+    <t>Discover or discern the existence, presence, or fact of an intrusion into information systems.</t>
   </si>
   <si>
     <t>D1 - Detect</t>
@@ -11315,7 +11315,7 @@
     <t>Deny</t>
   </si>
   <si>
-    <t>prevent disinformation creators from accessing and using critical information, systems, and services.</t>
+    <t xml:space="preserve">Prevent disinformation creators from accessing and using critical information, systems, and services. Deny is for an indefinite time period. </t>
   </si>
   <si>
     <t>D2 - Deny</t>
@@ -11327,7 +11327,7 @@
     <t>Disrupt</t>
   </si>
   <si>
-    <t>break or interrupt the flow of information.</t>
+    <t xml:space="preserve">Completely break or interrupt the flow of information, for a fixed amount of time. (Deny, for a limited time period).  Not allowing any efficacy, for a short amount of time. </t>
   </si>
   <si>
     <t>D3 - Disrupt</t>
@@ -11339,7 +11339,7 @@
     <t>Degrade</t>
   </si>
   <si>
-    <t>reduce the effectiveness or efficiency of adversary command and control or communications systems, and information collection efforts or means.</t>
+    <t xml:space="preserve">Reduce the effectiveness or efficiency of disinformation creators’ command and control or communications systems, and information collection efforts or means, either indefinitely, or for a limited time period. </t>
   </si>
   <si>
     <t>D4 - Degrade</t>
@@ -11351,7 +11351,7 @@
     <t>Deceive</t>
   </si>
   <si>
-    <t>cause a person to believe what is not true. military deception seeks to mislead adversary decision makers by manipulating their perception of reality.</t>
+    <t>Cause a person to believe what is not true. military deception seeks to mislead adversary decision makers by manipulating their perception of reality.</t>
   </si>
   <si>
     <t>D5 - Deceive</t>
@@ -11363,7 +11363,7 @@
     <t>Destroy</t>
   </si>
   <si>
-    <t>damage a system or entity so badly that it cannot perform any function or be restored to a usable condition without being entirely rebuilt.</t>
+    <t xml:space="preserve">Damage a system or entity so badly that it cannot perform any function or be restored to a usable condition without being entirely rebuilt. Destroy is permanent, e.g. you can rebuild a website, but it’s not the same website. </t>
   </si>
   <si>
     <t>D6 - Destroy</t>
@@ -11375,7 +11375,7 @@
     <t>Deter</t>
   </si>
   <si>
-    <t>discourage. We added Deter to the list as a potentially useful category too</t>
+    <t>Discourage.</t>
   </si>
   <si>
     <t>D7 - Deter</t>
@@ -12872,7 +12872,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="71">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -13563,6 +13563,21 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
         <color indexed="13"/>
       </right>
       <top style="thin">
@@ -13755,25 +13770,18 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -13786,15 +13794,22 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -14160,7 +14175,7 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -14202,22 +14217,19 @@
     <xf numFmtId="49" fontId="16" fillId="3" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="54" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="3" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="54" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="57" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -14226,19 +14238,22 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="59" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="59" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="60" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="62" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -14253,13 +14268,13 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="62" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="16" fillId="3" borderId="63" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="63" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="64" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="64" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="65" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -14319,18 +14334,6 @@
     <xf numFmtId="49" fontId="3" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="65" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="66" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="67" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -14340,10 +14343,13 @@
     <xf numFmtId="49" fontId="3" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="66" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="60" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -14358,7 +14364,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="68" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="67" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -14370,7 +14376,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="69" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="68" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -14406,7 +14415,13 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="69" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="70" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="71" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -16029,17 +16044,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" width="16.3516" style="165" customWidth="1"/>
-    <col min="3" max="3" width="47" style="165" customWidth="1"/>
+    <col min="3" max="3" width="107.242" style="165" customWidth="1"/>
     <col min="4" max="4" width="14.8516" style="165" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="165" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="165" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="165" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -16055,7 +16069,6 @@
       <c r="D1" t="s" s="166">
         <v>61</v>
       </c>
-      <c r="E1" s="168"/>
     </row>
     <row r="2" ht="46.65" customHeight="1">
       <c r="A2" t="s" s="96">
@@ -16071,7 +16084,6 @@
         <f>A2&amp;" - "&amp;B2</f>
         <v>2179</v>
       </c>
-      <c r="E2" s="169"/>
     </row>
     <row r="3" ht="24.65" customHeight="1">
       <c r="A3" t="s" s="96">
@@ -16087,9 +16099,8 @@
         <f>A3&amp;" - "&amp;B3</f>
         <v>2183</v>
       </c>
-      <c r="E3" s="169"/>
-    </row>
-    <row r="4" ht="14.7" customHeight="1">
+    </row>
+    <row r="4" ht="29.9" customHeight="1">
       <c r="A4" t="s" s="96">
         <v>2184</v>
       </c>
@@ -16103,7 +16114,6 @@
         <f>A4&amp;" - "&amp;B4</f>
         <v>2187</v>
       </c>
-      <c r="E4" s="169"/>
     </row>
     <row r="5" ht="35.65" customHeight="1">
       <c r="A5" t="s" s="96">
@@ -16119,7 +16129,6 @@
         <f>A5&amp;" - "&amp;B5</f>
         <v>2191</v>
       </c>
-      <c r="E5" s="169"/>
     </row>
     <row r="6" ht="35.65" customHeight="1">
       <c r="A6" t="s" s="96">
@@ -16135,7 +16144,6 @@
         <f>A6&amp;" - "&amp;B6</f>
         <v>2195</v>
       </c>
-      <c r="E6" s="169"/>
     </row>
     <row r="7" ht="35.65" customHeight="1">
       <c r="A7" t="s" s="96">
@@ -16151,7 +16159,6 @@
         <f>A7&amp;" - "&amp;B7</f>
         <v>2199</v>
       </c>
-      <c r="E7" s="169"/>
     </row>
     <row r="8" ht="24.65" customHeight="1">
       <c r="A8" t="s" s="96">
@@ -16167,21 +16174,6 @@
         <f>A8&amp;" - "&amp;B8</f>
         <v>2203</v>
       </c>
-      <c r="E8" s="169"/>
-    </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="170"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="171"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="68"/>
-    </row>
-    <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="69"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -16203,250 +16195,250 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="172" customWidth="1"/>
-    <col min="2" max="2" width="19.8516" style="172" customWidth="1"/>
-    <col min="3" max="3" width="58.3516" style="172" customWidth="1"/>
-    <col min="4" max="4" width="21.6719" style="172" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="172" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="172" customWidth="1"/>
+    <col min="1" max="1" width="8.5" style="168" customWidth="1"/>
+    <col min="2" max="2" width="19.8516" style="168" customWidth="1"/>
+    <col min="3" max="3" width="58.3516" style="168" customWidth="1"/>
+    <col min="4" max="4" width="21.6719" style="168" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="168" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="168" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="173">
+      <c r="A1" t="s" s="169">
         <v>57</v>
       </c>
-      <c r="B1" t="s" s="173">
+      <c r="B1" t="s" s="169">
         <v>58</v>
       </c>
-      <c r="C1" t="s" s="174">
+      <c r="C1" t="s" s="170">
         <v>60</v>
       </c>
-      <c r="D1" t="s" s="173">
+      <c r="D1" t="s" s="169">
         <v>61</v>
       </c>
-      <c r="E1" s="168"/>
+      <c r="E1" s="171"/>
     </row>
     <row r="2" ht="24.65" customHeight="1">
-      <c r="A2" t="s" s="175">
+      <c r="A2" t="s" s="172">
         <v>2204</v>
       </c>
-      <c r="B2" t="s" s="176">
+      <c r="B2" t="s" s="173">
         <v>2205</v>
       </c>
-      <c r="C2" t="s" s="176">
+      <c r="C2" t="s" s="173">
         <v>2206</v>
       </c>
-      <c r="D2" t="s" s="176">
+      <c r="D2" t="s" s="173">
         <f>A2&amp;" - "&amp;B2</f>
         <v>2207</v>
       </c>
-      <c r="E2" s="177"/>
+      <c r="E2" s="174"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="178">
+      <c r="A3" t="s" s="175">
         <v>2208</v>
       </c>
-      <c r="B3" t="s" s="179">
+      <c r="B3" t="s" s="176">
         <v>2209</v>
       </c>
-      <c r="C3" t="s" s="179">
+      <c r="C3" t="s" s="176">
         <v>2210</v>
       </c>
-      <c r="D3" t="s" s="179">
+      <c r="D3" t="s" s="176">
         <f>A3&amp;" - "&amp;B3</f>
         <v>2211</v>
       </c>
-      <c r="E3" s="177"/>
+      <c r="E3" s="174"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="178">
+      <c r="A4" t="s" s="175">
         <v>2212</v>
       </c>
-      <c r="B4" t="s" s="179">
+      <c r="B4" t="s" s="176">
         <v>853</v>
       </c>
-      <c r="C4" t="s" s="179">
+      <c r="C4" t="s" s="176">
         <v>2213</v>
       </c>
-      <c r="D4" t="s" s="179">
+      <c r="D4" t="s" s="176">
         <f>A4&amp;" - "&amp;B4</f>
         <v>2214</v>
       </c>
-      <c r="E4" s="177"/>
+      <c r="E4" s="174"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="178">
+      <c r="A5" t="s" s="175">
         <v>2215</v>
       </c>
-      <c r="B5" t="s" s="179">
+      <c r="B5" t="s" s="176">
         <v>2216</v>
       </c>
-      <c r="C5" t="s" s="179">
+      <c r="C5" t="s" s="176">
         <v>2217</v>
       </c>
-      <c r="D5" t="s" s="179">
+      <c r="D5" t="s" s="176">
         <f>A5&amp;" - "&amp;B5</f>
         <v>2218</v>
       </c>
-      <c r="E5" s="177"/>
+      <c r="E5" s="174"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="178">
+      <c r="A6" t="s" s="175">
         <v>2219</v>
       </c>
-      <c r="B6" t="s" s="179">
+      <c r="B6" t="s" s="176">
         <v>2220</v>
       </c>
-      <c r="C6" t="s" s="179">
+      <c r="C6" t="s" s="176">
         <v>2221</v>
       </c>
-      <c r="D6" t="s" s="179">
+      <c r="D6" t="s" s="176">
         <f>A6&amp;" - "&amp;B6</f>
         <v>2222</v>
       </c>
-      <c r="E6" s="177"/>
+      <c r="E6" s="174"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="178">
+      <c r="A7" t="s" s="175">
         <v>2223</v>
       </c>
-      <c r="B7" t="s" s="179">
+      <c r="B7" t="s" s="176">
         <v>2224</v>
       </c>
-      <c r="C7" t="s" s="179">
+      <c r="C7" t="s" s="176">
         <v>2225</v>
       </c>
-      <c r="D7" t="s" s="179">
+      <c r="D7" t="s" s="176">
         <f>A7&amp;" - "&amp;B7</f>
         <v>2226</v>
       </c>
-      <c r="E7" s="177"/>
+      <c r="E7" s="174"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="178">
+      <c r="A8" t="s" s="175">
         <v>2227</v>
       </c>
-      <c r="B8" t="s" s="179">
+      <c r="B8" t="s" s="176">
         <v>463</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" t="s" s="179">
+      <c r="C8" s="177"/>
+      <c r="D8" t="s" s="176">
         <f>A8&amp;" - "&amp;B8</f>
         <v>2228</v>
       </c>
-      <c r="E8" s="177"/>
+      <c r="E8" s="174"/>
     </row>
     <row r="9" ht="24.65" customHeight="1">
-      <c r="A9" t="s" s="178">
+      <c r="A9" t="s" s="175">
         <v>2229</v>
       </c>
-      <c r="B9" t="s" s="179">
+      <c r="B9" t="s" s="176">
         <v>2230</v>
       </c>
-      <c r="C9" t="s" s="179">
+      <c r="C9" t="s" s="176">
         <v>2231</v>
       </c>
-      <c r="D9" t="s" s="179">
+      <c r="D9" t="s" s="176">
         <f>A9&amp;" - "&amp;B9</f>
         <v>2232</v>
       </c>
-      <c r="E9" s="177"/>
+      <c r="E9" s="174"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="178">
+      <c r="A10" t="s" s="175">
         <v>2233</v>
       </c>
-      <c r="B10" t="s" s="179">
+      <c r="B10" t="s" s="176">
         <v>2234</v>
       </c>
-      <c r="C10" t="s" s="179">
+      <c r="C10" t="s" s="176">
         <v>2235</v>
       </c>
-      <c r="D10" t="s" s="179">
+      <c r="D10" t="s" s="176">
         <f>A10&amp;" - "&amp;B10</f>
         <v>2236</v>
       </c>
-      <c r="E10" s="177"/>
+      <c r="E10" s="174"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" t="s" s="178">
+      <c r="A11" t="s" s="175">
         <v>2237</v>
       </c>
-      <c r="B11" t="s" s="179">
+      <c r="B11" t="s" s="176">
         <v>2238</v>
       </c>
-      <c r="C11" t="s" s="179">
+      <c r="C11" t="s" s="176">
         <v>2239</v>
       </c>
-      <c r="D11" t="s" s="179">
+      <c r="D11" t="s" s="176">
         <f>A11&amp;" - "&amp;B11</f>
         <v>2240</v>
       </c>
-      <c r="E11" s="177"/>
+      <c r="E11" s="174"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" t="s" s="178">
+      <c r="A12" t="s" s="175">
         <v>2241</v>
       </c>
-      <c r="B12" t="s" s="179">
+      <c r="B12" t="s" s="176">
         <v>2242</v>
       </c>
-      <c r="C12" t="s" s="179">
+      <c r="C12" t="s" s="176">
         <v>2243</v>
       </c>
-      <c r="D12" t="s" s="179">
+      <c r="D12" t="s" s="176">
         <f>A12&amp;" - "&amp;B12</f>
         <v>2244</v>
       </c>
-      <c r="E12" s="177"/>
+      <c r="E12" s="174"/>
     </row>
     <row r="13" ht="24.65" customHeight="1">
-      <c r="A13" t="s" s="178">
+      <c r="A13" t="s" s="175">
         <v>2245</v>
       </c>
-      <c r="B13" t="s" s="179">
+      <c r="B13" t="s" s="176">
         <v>2246</v>
       </c>
-      <c r="C13" t="s" s="179">
+      <c r="C13" t="s" s="176">
         <v>2247</v>
       </c>
-      <c r="D13" t="s" s="179">
+      <c r="D13" t="s" s="176">
         <f>A13&amp;" - "&amp;B13</f>
         <v>2248</v>
       </c>
-      <c r="E13" s="177"/>
+      <c r="E13" s="174"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" t="s" s="178">
+      <c r="A14" t="s" s="175">
         <v>2249</v>
       </c>
-      <c r="B14" t="s" s="179">
+      <c r="B14" t="s" s="176">
         <v>2250</v>
       </c>
-      <c r="C14" t="s" s="179">
+      <c r="C14" t="s" s="176">
         <v>2251</v>
       </c>
-      <c r="D14" t="s" s="179">
+      <c r="D14" t="s" s="176">
         <f>A14&amp;" - "&amp;B14</f>
         <v>2252</v>
       </c>
-      <c r="E14" s="177"/>
+      <c r="E14" s="174"/>
     </row>
     <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" t="s" s="178">
+      <c r="A15" t="s" s="175">
         <v>2253</v>
       </c>
-      <c r="B15" t="s" s="179">
+      <c r="B15" t="s" s="176">
         <v>2254</v>
       </c>
-      <c r="C15" t="s" s="179">
+      <c r="C15" t="s" s="176">
         <v>2255</v>
       </c>
-      <c r="D15" t="s" s="179">
+      <c r="D15" t="s" s="176">
         <f>A15&amp;" - "&amp;B15</f>
         <v>2256</v>
       </c>
-      <c r="E15" s="181"/>
+      <c r="E15" s="178"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -16468,31 +16460,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.85156" style="182" customWidth="1"/>
-    <col min="2" max="2" width="28" style="182" customWidth="1"/>
-    <col min="3" max="3" width="35" style="182" customWidth="1"/>
-    <col min="4" max="5" width="20.1719" style="182" customWidth="1"/>
-    <col min="6" max="6" width="31.8516" style="182" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="182" customWidth="1"/>
+    <col min="1" max="1" width="6.85156" style="179" customWidth="1"/>
+    <col min="2" max="2" width="28" style="179" customWidth="1"/>
+    <col min="3" max="3" width="35" style="179" customWidth="1"/>
+    <col min="4" max="5" width="20.1719" style="179" customWidth="1"/>
+    <col min="6" max="6" width="31.8516" style="179" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="179" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="183">
+      <c r="A1" t="s" s="180">
         <v>57</v>
       </c>
-      <c r="B1" t="s" s="183">
+      <c r="B1" t="s" s="180">
         <v>58</v>
       </c>
-      <c r="C1" t="s" s="183">
+      <c r="C1" t="s" s="180">
         <v>60</v>
       </c>
-      <c r="D1" t="s" s="183">
+      <c r="D1" t="s" s="180">
         <v>2257</v>
       </c>
-      <c r="E1" t="s" s="183">
+      <c r="E1" t="s" s="180">
         <v>2258</v>
       </c>
-      <c r="F1" t="s" s="183">
+      <c r="F1" t="s" s="180">
         <v>61</v>
       </c>
     </row>
@@ -17163,12 +17155,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.85156" style="184" customWidth="1"/>
-    <col min="2" max="2" width="21.1719" style="184" customWidth="1"/>
-    <col min="3" max="3" width="35" style="184" customWidth="1"/>
-    <col min="4" max="4" width="20.1719" style="184" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="184" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="184" customWidth="1"/>
+    <col min="1" max="1" width="6.85156" style="181" customWidth="1"/>
+    <col min="2" max="2" width="21.1719" style="181" customWidth="1"/>
+    <col min="3" max="3" width="35" style="181" customWidth="1"/>
+    <col min="4" max="4" width="20.1719" style="181" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="181" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="181" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -17184,7 +17176,7 @@
       <c r="D1" t="s" s="166">
         <v>61</v>
       </c>
-      <c r="E1" s="168"/>
+      <c r="E1" s="171"/>
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="96">
@@ -17198,7 +17190,7 @@
         <f>A2&amp;" - "&amp;B2</f>
         <v>2366</v>
       </c>
-      <c r="E2" s="169"/>
+      <c r="E2" s="182"/>
     </row>
     <row r="3" ht="14.7" customHeight="1">
       <c r="A3" t="s" s="96">
@@ -17212,7 +17204,7 @@
         <f>A3&amp;" - "&amp;B3</f>
         <v>2367</v>
       </c>
-      <c r="E3" s="169"/>
+      <c r="E3" s="182"/>
     </row>
     <row r="4" ht="26.7" customHeight="1">
       <c r="A4" t="s" s="96">
@@ -17226,7 +17218,7 @@
         <f>A4&amp;" - "&amp;B4</f>
         <v>2368</v>
       </c>
-      <c r="E4" s="169"/>
+      <c r="E4" s="182"/>
     </row>
     <row r="5" ht="14.7" customHeight="1">
       <c r="A5" t="s" s="96">
@@ -17240,7 +17232,7 @@
         <f>A5&amp;" - "&amp;B5</f>
         <v>2370</v>
       </c>
-      <c r="E5" s="169"/>
+      <c r="E5" s="182"/>
     </row>
     <row r="6" ht="14.7" customHeight="1">
       <c r="A6" t="s" s="96">
@@ -17254,7 +17246,7 @@
         <f>A6&amp;" - "&amp;B6</f>
         <v>2372</v>
       </c>
-      <c r="E6" s="169"/>
+      <c r="E6" s="182"/>
     </row>
     <row r="7" ht="26.7" customHeight="1">
       <c r="A7" t="s" s="96">
@@ -17268,7 +17260,7 @@
         <f>A7&amp;" - "&amp;B7</f>
         <v>2373</v>
       </c>
-      <c r="E7" s="169"/>
+      <c r="E7" s="182"/>
     </row>
     <row r="8" ht="26.7" customHeight="1">
       <c r="A8" t="s" s="96">
@@ -17282,7 +17274,7 @@
         <f>A8&amp;" - "&amp;B8</f>
         <v>2374</v>
       </c>
-      <c r="E8" s="169"/>
+      <c r="E8" s="182"/>
     </row>
     <row r="9" ht="26.7" customHeight="1">
       <c r="A9" t="s" s="96">
@@ -17296,7 +17288,7 @@
         <f>A9&amp;" - "&amp;B9</f>
         <v>2375</v>
       </c>
-      <c r="E9" s="169"/>
+      <c r="E9" s="182"/>
     </row>
     <row r="10" ht="14.7" customHeight="1">
       <c r="A10" t="s" s="96">
@@ -17310,7 +17302,7 @@
         <f>A10&amp;" - "&amp;B10</f>
         <v>2376</v>
       </c>
-      <c r="E10" s="169"/>
+      <c r="E10" s="182"/>
     </row>
     <row r="11" ht="14.7" customHeight="1">
       <c r="A11" t="s" s="96">
@@ -17324,7 +17316,7 @@
         <f>A11&amp;" - "&amp;B11</f>
         <v>2377</v>
       </c>
-      <c r="E11" s="185"/>
+      <c r="E11" s="183"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -17346,33 +17338,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.35156" style="186" customWidth="1"/>
-    <col min="2" max="2" width="23.3516" style="186" customWidth="1"/>
-    <col min="3" max="3" width="26.6719" style="186" customWidth="1"/>
-    <col min="4" max="4" width="20.6719" style="186" customWidth="1"/>
-    <col min="5" max="5" width="29.1719" style="186" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="186" customWidth="1"/>
+    <col min="1" max="1" width="8.35156" style="184" customWidth="1"/>
+    <col min="2" max="2" width="23.3516" style="184" customWidth="1"/>
+    <col min="3" max="3" width="26.6719" style="184" customWidth="1"/>
+    <col min="4" max="4" width="20.6719" style="184" customWidth="1"/>
+    <col min="5" max="5" width="29.1719" style="184" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="184" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" customHeight="1">
-      <c r="A1" t="s" s="187">
+      <c r="A1" t="s" s="185">
         <v>57</v>
       </c>
-      <c r="B1" t="s" s="187">
+      <c r="B1" t="s" s="185">
         <v>58</v>
       </c>
-      <c r="C1" t="s" s="187">
+      <c r="C1" t="s" s="185">
         <v>60</v>
       </c>
-      <c r="D1" t="s" s="187">
+      <c r="D1" t="s" s="185">
         <v>2378</v>
       </c>
-      <c r="E1" t="s" s="187">
+      <c r="E1" t="s" s="185">
         <v>61</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="188">
+      <c r="A2" t="s" s="186">
         <v>2379</v>
       </c>
       <c r="B2" t="s" s="56">
@@ -17390,7 +17382,7 @@
       </c>
     </row>
     <row r="3" ht="26.05" customHeight="1">
-      <c r="A3" t="s" s="189">
+      <c r="A3" t="s" s="187">
         <v>2384</v>
       </c>
       <c r="B3" t="s" s="60">
@@ -17408,7 +17400,7 @@
       </c>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" t="s" s="189">
+      <c r="A4" t="s" s="187">
         <v>2389</v>
       </c>
       <c r="B4" t="s" s="60">
@@ -17426,7 +17418,7 @@
       </c>
     </row>
     <row r="5" ht="26.05" customHeight="1">
-      <c r="A5" t="s" s="189">
+      <c r="A5" t="s" s="187">
         <v>2393</v>
       </c>
       <c r="B5" t="s" s="60">
@@ -17444,7 +17436,7 @@
       </c>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" t="s" s="189">
+      <c r="A6" t="s" s="187">
         <v>2398</v>
       </c>
       <c r="B6" t="s" s="60">
@@ -17462,7 +17454,7 @@
       </c>
     </row>
     <row r="7" ht="26.05" customHeight="1">
-      <c r="A7" t="s" s="189">
+      <c r="A7" t="s" s="187">
         <v>2402</v>
       </c>
       <c r="B7" t="s" s="60">
@@ -17520,156 +17512,156 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="11" width="16.3516" style="190" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="190" customWidth="1"/>
+    <col min="1" max="11" width="16.3516" style="188" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="188" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="173">
+      <c r="A1" t="s" s="169">
         <v>57</v>
       </c>
-      <c r="B1" t="s" s="173">
+      <c r="B1" t="s" s="169">
         <v>2405</v>
       </c>
-      <c r="C1" t="s" s="173">
+      <c r="C1" t="s" s="169">
         <v>2406</v>
       </c>
-      <c r="D1" t="s" s="173">
+      <c r="D1" t="s" s="169">
         <v>2407</v>
       </c>
-      <c r="E1" t="s" s="173">
+      <c r="E1" t="s" s="169">
         <v>58</v>
       </c>
-      <c r="F1" t="s" s="174">
+      <c r="F1" t="s" s="170">
         <v>2408</v>
       </c>
-      <c r="G1" t="s" s="173">
+      <c r="G1" t="s" s="169">
         <v>2409</v>
       </c>
-      <c r="H1" t="s" s="173">
+      <c r="H1" t="s" s="169">
         <v>470</v>
       </c>
-      <c r="I1" t="s" s="173">
+      <c r="I1" t="s" s="169">
         <v>2410</v>
       </c>
-      <c r="J1" t="s" s="173">
+      <c r="J1" t="s" s="169">
         <v>60</v>
       </c>
-      <c r="K1" t="s" s="173">
+      <c r="K1" t="s" s="169">
         <v>61</v>
       </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="191">
+      <c r="A2" t="s" s="189">
         <v>2411</v>
       </c>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="194"/>
-      <c r="G2" t="s" s="191">
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="190"/>
+      <c r="F2" s="192"/>
+      <c r="G2" t="s" s="189">
         <v>2412</v>
       </c>
-      <c r="H2" t="s" s="191">
+      <c r="H2" t="s" s="189">
         <v>2413</v>
       </c>
-      <c r="I2" t="s" s="195">
+      <c r="I2" t="s" s="193">
         <v>2414</v>
       </c>
-      <c r="J2" s="192"/>
-      <c r="K2" t="s" s="191">
+      <c r="J2" s="190"/>
+      <c r="K2" t="s" s="189">
         <f>A2</f>
         <v>2415</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="191">
+      <c r="A3" t="s" s="189">
         <v>2416</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="194"/>
-      <c r="G3" t="s" s="191">
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="192"/>
+      <c r="G3" t="s" s="189">
         <v>2417</v>
       </c>
-      <c r="H3" t="s" s="191">
+      <c r="H3" t="s" s="189">
         <v>1004</v>
       </c>
-      <c r="I3" t="s" s="195">
+      <c r="I3" t="s" s="193">
         <v>2418</v>
       </c>
-      <c r="J3" s="192"/>
-      <c r="K3" t="s" s="191">
+      <c r="J3" s="190"/>
+      <c r="K3" t="s" s="189">
         <f>A3</f>
         <v>2419</v>
       </c>
     </row>
     <row r="4" ht="200.65" customHeight="1">
-      <c r="A4" t="s" s="191">
+      <c r="A4" t="s" s="189">
         <v>2420</v>
       </c>
-      <c r="B4" s="192"/>
-      <c r="C4" s="192"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="192"/>
-      <c r="F4" t="s" s="196">
+      <c r="B4" s="190"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="190"/>
+      <c r="F4" t="s" s="194">
         <v>2421</v>
       </c>
-      <c r="G4" t="s" s="191">
+      <c r="G4" t="s" s="189">
         <v>2417</v>
       </c>
-      <c r="H4" t="s" s="191">
+      <c r="H4" t="s" s="189">
         <v>1004</v>
       </c>
-      <c r="I4" t="s" s="195">
+      <c r="I4" t="s" s="193">
         <v>2422</v>
       </c>
-      <c r="J4" s="192"/>
-      <c r="K4" t="s" s="191">
+      <c r="J4" s="190"/>
+      <c r="K4" t="s" s="189">
         <f>A4</f>
         <v>2423</v>
       </c>
     </row>
     <row r="5" ht="68.65" customHeight="1">
-      <c r="A5" t="s" s="191">
+      <c r="A5" t="s" s="189">
         <v>2424</v>
       </c>
-      <c r="B5" s="192"/>
-      <c r="C5" s="192"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="192"/>
-      <c r="F5" t="s" s="196">
+      <c r="B5" s="190"/>
+      <c r="C5" s="190"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="190"/>
+      <c r="F5" t="s" s="194">
         <v>2425</v>
       </c>
-      <c r="G5" t="s" s="191">
+      <c r="G5" t="s" s="189">
         <v>2426</v>
       </c>
-      <c r="H5" t="s" s="191">
+      <c r="H5" t="s" s="189">
         <v>803</v>
       </c>
-      <c r="I5" t="s" s="195">
+      <c r="I5" t="s" s="193">
         <v>652</v>
       </c>
-      <c r="J5" s="192"/>
-      <c r="K5" t="s" s="191">
+      <c r="J5" s="190"/>
+      <c r="K5" t="s" s="189">
         <f>A5</f>
         <v>2427</v>
       </c>
     </row>
     <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="170"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="171"/>
-      <c r="G6" s="171"/>
-      <c r="H6" s="171"/>
-      <c r="I6" s="171"/>
-      <c r="J6" s="171"/>
+      <c r="A6" s="195"/>
+      <c r="B6" s="196"/>
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="196"/>
+      <c r="F6" s="196"/>
+      <c r="G6" s="196"/>
+      <c r="H6" s="196"/>
+      <c r="I6" s="196"/>
+      <c r="J6" s="196"/>
       <c r="K6" s="197"/>
     </row>
     <row r="7" ht="14.7" customHeight="1">
@@ -17762,10 +17754,10 @@
       <c r="A1" t="s" s="199">
         <v>57</v>
       </c>
-      <c r="B1" t="s" s="173">
+      <c r="B1" t="s" s="169">
         <v>2405</v>
       </c>
-      <c r="C1" t="s" s="173">
+      <c r="C1" t="s" s="169">
         <v>2428</v>
       </c>
       <c r="D1" s="200"/>
@@ -17785,17 +17777,17 @@
       <c r="A2" t="s" s="202">
         <v>2429</v>
       </c>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" t="s" s="191">
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E2" t="s" s="195">
+      <c r="E2" t="s" s="193">
         <v>2431</v>
       </c>
-      <c r="F2" s="193"/>
-      <c r="G2" s="193"/>
-      <c r="H2" s="194"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="192"/>
       <c r="I2" t="s" s="203">
         <f>A2</f>
         <v>2432</v>
@@ -17805,17 +17797,17 @@
       <c r="A3" t="s" s="202">
         <v>2433</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" t="s" s="191">
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E3" t="s" s="195">
+      <c r="E3" t="s" s="193">
         <v>2434</v>
       </c>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="194"/>
+      <c r="F3" s="191"/>
+      <c r="G3" s="191"/>
+      <c r="H3" s="192"/>
       <c r="I3" t="s" s="203">
         <f>A3</f>
         <v>2435</v>
@@ -17825,17 +17817,17 @@
       <c r="A4" t="s" s="202">
         <v>2436</v>
       </c>
-      <c r="B4" s="192"/>
-      <c r="C4" s="192"/>
-      <c r="D4" t="s" s="191">
+      <c r="B4" s="190"/>
+      <c r="C4" s="190"/>
+      <c r="D4" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E4" t="s" s="195">
+      <c r="E4" t="s" s="193">
         <v>5</v>
       </c>
-      <c r="F4" s="193"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="194"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="192"/>
       <c r="I4" t="s" s="203">
         <f>A4</f>
         <v>2437</v>
@@ -17845,17 +17837,17 @@
       <c r="A5" t="s" s="202">
         <v>2438</v>
       </c>
-      <c r="B5" s="192"/>
-      <c r="C5" s="192"/>
-      <c r="D5" t="s" s="191">
+      <c r="B5" s="190"/>
+      <c r="C5" s="190"/>
+      <c r="D5" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E5" t="s" s="195">
+      <c r="E5" t="s" s="193">
         <v>2439</v>
       </c>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="194"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="192"/>
       <c r="I5" t="s" s="203">
         <f>A5</f>
         <v>2440</v>
@@ -17865,17 +17857,17 @@
       <c r="A6" t="s" s="202">
         <v>2441</v>
       </c>
-      <c r="B6" s="192"/>
-      <c r="C6" s="192"/>
-      <c r="D6" t="s" s="191">
+      <c r="B6" s="190"/>
+      <c r="C6" s="190"/>
+      <c r="D6" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E6" t="s" s="195">
+      <c r="E6" t="s" s="193">
         <v>2442</v>
       </c>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="194"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="191"/>
+      <c r="H6" s="192"/>
       <c r="I6" t="s" s="203">
         <f>A6</f>
         <v>2443</v>
@@ -17885,17 +17877,17 @@
       <c r="A7" t="s" s="202">
         <v>2444</v>
       </c>
-      <c r="B7" s="192"/>
-      <c r="C7" s="192"/>
-      <c r="D7" t="s" s="191">
+      <c r="B7" s="190"/>
+      <c r="C7" s="190"/>
+      <c r="D7" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E7" t="s" s="195">
+      <c r="E7" t="s" s="193">
         <v>2445</v>
       </c>
-      <c r="F7" s="193"/>
-      <c r="G7" s="193"/>
-      <c r="H7" s="194"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="192"/>
       <c r="I7" t="s" s="203">
         <f>A7</f>
         <v>2446</v>
@@ -17905,17 +17897,17 @@
       <c r="A8" t="s" s="202">
         <v>2447</v>
       </c>
-      <c r="B8" s="192"/>
-      <c r="C8" s="192"/>
-      <c r="D8" t="s" s="191">
+      <c r="B8" s="190"/>
+      <c r="C8" s="190"/>
+      <c r="D8" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E8" t="s" s="195">
+      <c r="E8" t="s" s="193">
         <v>2448</v>
       </c>
-      <c r="F8" s="193"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="194"/>
+      <c r="F8" s="191"/>
+      <c r="G8" s="191"/>
+      <c r="H8" s="192"/>
       <c r="I8" t="s" s="203">
         <f>A8</f>
         <v>2449</v>
@@ -17925,17 +17917,17 @@
       <c r="A9" t="s" s="202">
         <v>2450</v>
       </c>
-      <c r="B9" s="192"/>
-      <c r="C9" s="192"/>
-      <c r="D9" t="s" s="191">
+      <c r="B9" s="190"/>
+      <c r="C9" s="190"/>
+      <c r="D9" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E9" t="s" s="195">
+      <c r="E9" t="s" s="193">
         <v>2451</v>
       </c>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" t="s" s="196">
+      <c r="F9" s="191"/>
+      <c r="G9" s="191"/>
+      <c r="H9" t="s" s="194">
         <v>2452</v>
       </c>
       <c r="I9" t="s" s="203">
@@ -17947,17 +17939,17 @@
       <c r="A10" t="s" s="202">
         <v>2454</v>
       </c>
-      <c r="B10" s="192"/>
-      <c r="C10" s="192"/>
-      <c r="D10" t="s" s="191">
+      <c r="B10" s="190"/>
+      <c r="C10" s="190"/>
+      <c r="D10" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E10" t="s" s="195">
+      <c r="E10" t="s" s="193">
         <v>2455</v>
       </c>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="194"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="191"/>
+      <c r="H10" s="192"/>
       <c r="I10" t="s" s="203">
         <f>A10</f>
         <v>2456</v>
@@ -17967,17 +17959,17 @@
       <c r="A11" t="s" s="202">
         <v>2457</v>
       </c>
-      <c r="B11" s="192"/>
-      <c r="C11" s="192"/>
-      <c r="D11" t="s" s="191">
+      <c r="B11" s="190"/>
+      <c r="C11" s="190"/>
+      <c r="D11" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E11" t="s" s="195">
+      <c r="E11" t="s" s="193">
         <v>2458</v>
       </c>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" t="s" s="196">
+      <c r="F11" s="191"/>
+      <c r="G11" s="191"/>
+      <c r="H11" t="s" s="194">
         <v>2459</v>
       </c>
       <c r="I11" t="s" s="203">
@@ -17989,17 +17981,17 @@
       <c r="A12" t="s" s="202">
         <v>2461</v>
       </c>
-      <c r="B12" s="192"/>
-      <c r="C12" s="192"/>
-      <c r="D12" t="s" s="191">
+      <c r="B12" s="190"/>
+      <c r="C12" s="190"/>
+      <c r="D12" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E12" t="s" s="195">
+      <c r="E12" t="s" s="193">
         <v>2462</v>
       </c>
-      <c r="F12" s="193"/>
-      <c r="G12" s="193"/>
-      <c r="H12" t="s" s="196">
+      <c r="F12" s="191"/>
+      <c r="G12" s="191"/>
+      <c r="H12" t="s" s="194">
         <v>2463</v>
       </c>
       <c r="I12" t="s" s="203">
@@ -18011,17 +18003,17 @@
       <c r="A13" t="s" s="202">
         <v>2465</v>
       </c>
-      <c r="B13" s="192"/>
-      <c r="C13" s="192"/>
-      <c r="D13" t="s" s="191">
+      <c r="B13" s="190"/>
+      <c r="C13" s="190"/>
+      <c r="D13" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E13" t="s" s="195">
+      <c r="E13" t="s" s="193">
         <v>2466</v>
       </c>
-      <c r="F13" s="193"/>
-      <c r="G13" s="193"/>
-      <c r="H13" s="194"/>
+      <c r="F13" s="191"/>
+      <c r="G13" s="191"/>
+      <c r="H13" s="192"/>
       <c r="I13" t="s" s="203">
         <f>A13</f>
         <v>2467</v>
@@ -18031,17 +18023,17 @@
       <c r="A14" t="s" s="202">
         <v>2468</v>
       </c>
-      <c r="B14" s="192"/>
-      <c r="C14" s="192"/>
-      <c r="D14" t="s" s="191">
+      <c r="B14" s="190"/>
+      <c r="C14" s="190"/>
+      <c r="D14" t="s" s="189">
         <v>2430</v>
       </c>
-      <c r="E14" t="s" s="195">
+      <c r="E14" t="s" s="193">
         <v>2469</v>
       </c>
-      <c r="F14" s="193"/>
-      <c r="G14" s="193"/>
-      <c r="H14" s="194"/>
+      <c r="F14" s="191"/>
+      <c r="G14" s="191"/>
+      <c r="H14" s="192"/>
       <c r="I14" t="s" s="203">
         <f>A14</f>
         <v>2470</v>
@@ -18051,13 +18043,13 @@
       <c r="A15" t="s" s="202">
         <v>2471</v>
       </c>
-      <c r="B15" s="192"/>
-      <c r="C15" s="192"/>
-      <c r="D15" s="193"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="193"/>
-      <c r="G15" s="193"/>
-      <c r="H15" s="194"/>
+      <c r="B15" s="190"/>
+      <c r="C15" s="190"/>
+      <c r="D15" s="191"/>
+      <c r="E15" s="190"/>
+      <c r="F15" s="191"/>
+      <c r="G15" s="191"/>
+      <c r="H15" s="192"/>
       <c r="I15" t="s" s="203">
         <f>A15</f>
         <v>2472</v>
@@ -18067,15 +18059,15 @@
       <c r="A16" t="s" s="202">
         <v>2473</v>
       </c>
-      <c r="B16" s="192"/>
-      <c r="C16" s="192"/>
-      <c r="D16" s="193"/>
+      <c r="B16" s="190"/>
+      <c r="C16" s="190"/>
+      <c r="D16" s="191"/>
       <c r="E16" t="s" s="120">
         <v>2474</v>
       </c>
-      <c r="F16" s="193"/>
-      <c r="G16" s="193"/>
-      <c r="H16" s="194"/>
+      <c r="F16" s="191"/>
+      <c r="G16" s="191"/>
+      <c r="H16" s="192"/>
       <c r="I16" t="s" s="203">
         <f>A16</f>
         <v>2475</v>
@@ -18085,15 +18077,15 @@
       <c r="A17" t="s" s="202">
         <v>2476</v>
       </c>
-      <c r="B17" s="192"/>
-      <c r="C17" s="192"/>
-      <c r="D17" s="193"/>
-      <c r="E17" t="s" s="195">
+      <c r="B17" s="190"/>
+      <c r="C17" s="190"/>
+      <c r="D17" s="191"/>
+      <c r="E17" t="s" s="193">
         <v>2477</v>
       </c>
-      <c r="F17" s="193"/>
-      <c r="G17" s="193"/>
-      <c r="H17" s="194"/>
+      <c r="F17" s="191"/>
+      <c r="G17" s="191"/>
+      <c r="H17" s="192"/>
       <c r="I17" t="s" s="203">
         <f>A17</f>
         <v>2478</v>
@@ -18103,17 +18095,17 @@
       <c r="A18" t="s" s="202">
         <v>2479</v>
       </c>
-      <c r="B18" s="192"/>
-      <c r="C18" s="192"/>
-      <c r="D18" t="s" s="191">
+      <c r="B18" s="190"/>
+      <c r="C18" s="190"/>
+      <c r="D18" t="s" s="189">
         <v>2480</v>
       </c>
-      <c r="E18" t="s" s="195">
+      <c r="E18" t="s" s="193">
         <v>2481</v>
       </c>
-      <c r="F18" s="193"/>
-      <c r="G18" s="193"/>
-      <c r="H18" s="194"/>
+      <c r="F18" s="191"/>
+      <c r="G18" s="191"/>
+      <c r="H18" s="192"/>
       <c r="I18" t="s" s="203">
         <f>A18</f>
         <v>2482</v>
@@ -18123,17 +18115,17 @@
       <c r="A19" t="s" s="202">
         <v>2483</v>
       </c>
-      <c r="B19" s="192"/>
-      <c r="C19" s="192"/>
-      <c r="D19" t="s" s="191">
+      <c r="B19" s="190"/>
+      <c r="C19" s="190"/>
+      <c r="D19" t="s" s="189">
         <v>2480</v>
       </c>
       <c r="E19" t="s" s="120">
         <v>2484</v>
       </c>
-      <c r="F19" s="193"/>
-      <c r="G19" s="193"/>
-      <c r="H19" s="194"/>
+      <c r="F19" s="191"/>
+      <c r="G19" s="191"/>
+      <c r="H19" s="192"/>
       <c r="I19" t="s" s="203">
         <f>A19</f>
         <v>2485</v>
@@ -18143,13 +18135,13 @@
       <c r="A20" t="s" s="202">
         <v>2486</v>
       </c>
-      <c r="B20" s="192"/>
-      <c r="C20" s="192"/>
-      <c r="D20" s="193"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="193"/>
-      <c r="G20" s="193"/>
-      <c r="H20" s="194"/>
+      <c r="B20" s="190"/>
+      <c r="C20" s="190"/>
+      <c r="D20" s="191"/>
+      <c r="E20" s="190"/>
+      <c r="F20" s="191"/>
+      <c r="G20" s="191"/>
+      <c r="H20" s="192"/>
       <c r="I20" t="s" s="203">
         <f>A20</f>
         <v>2487</v>
@@ -18159,17 +18151,17 @@
       <c r="A21" t="s" s="202">
         <v>2488</v>
       </c>
-      <c r="B21" s="192"/>
-      <c r="C21" s="192"/>
-      <c r="D21" t="s" s="191">
+      <c r="B21" s="190"/>
+      <c r="C21" s="190"/>
+      <c r="D21" t="s" s="189">
         <v>2489</v>
       </c>
-      <c r="E21" t="s" s="195">
+      <c r="E21" t="s" s="193">
         <v>2490</v>
       </c>
-      <c r="F21" s="193"/>
-      <c r="G21" s="193"/>
-      <c r="H21" s="194"/>
+      <c r="F21" s="191"/>
+      <c r="G21" s="191"/>
+      <c r="H21" s="192"/>
       <c r="I21" t="s" s="203">
         <f>A21</f>
         <v>2491</v>
@@ -18179,17 +18171,17 @@
       <c r="A22" t="s" s="202">
         <v>2492</v>
       </c>
-      <c r="B22" s="192"/>
-      <c r="C22" s="192"/>
-      <c r="D22" t="s" s="191">
+      <c r="B22" s="190"/>
+      <c r="C22" s="190"/>
+      <c r="D22" t="s" s="189">
         <v>2489</v>
       </c>
-      <c r="E22" t="s" s="195">
+      <c r="E22" t="s" s="193">
         <v>2493</v>
       </c>
-      <c r="F22" s="193"/>
-      <c r="G22" s="193"/>
-      <c r="H22" s="194"/>
+      <c r="F22" s="191"/>
+      <c r="G22" s="191"/>
+      <c r="H22" s="192"/>
       <c r="I22" t="s" s="203">
         <f>A22</f>
         <v>2494</v>
@@ -18199,13 +18191,13 @@
       <c r="A23" t="s" s="202">
         <v>2495</v>
       </c>
-      <c r="B23" s="192"/>
-      <c r="C23" s="192"/>
-      <c r="D23" s="193"/>
-      <c r="E23" s="192"/>
-      <c r="F23" s="193"/>
-      <c r="G23" s="193"/>
-      <c r="H23" s="194"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="190"/>
+      <c r="D23" s="191"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="191"/>
+      <c r="G23" s="191"/>
+      <c r="H23" s="192"/>
       <c r="I23" t="s" s="203">
         <f>A23</f>
         <v>2496</v>
@@ -18215,13 +18207,13 @@
       <c r="A24" t="s" s="202">
         <v>2497</v>
       </c>
-      <c r="B24" s="192"/>
-      <c r="C24" s="192"/>
-      <c r="D24" s="193"/>
-      <c r="E24" s="192"/>
-      <c r="F24" s="193"/>
-      <c r="G24" s="193"/>
-      <c r="H24" s="194"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="190"/>
+      <c r="D24" s="191"/>
+      <c r="E24" s="190"/>
+      <c r="F24" s="191"/>
+      <c r="G24" s="191"/>
+      <c r="H24" s="192"/>
       <c r="I24" t="s" s="203">
         <f>A24</f>
         <v>2498</v>
@@ -18231,13 +18223,13 @@
       <c r="A25" t="s" s="202">
         <v>2499</v>
       </c>
-      <c r="B25" s="192"/>
-      <c r="C25" s="192"/>
-      <c r="D25" s="193"/>
-      <c r="E25" s="192"/>
-      <c r="F25" s="193"/>
-      <c r="G25" s="193"/>
-      <c r="H25" s="194"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="190"/>
+      <c r="D25" s="191"/>
+      <c r="E25" s="190"/>
+      <c r="F25" s="191"/>
+      <c r="G25" s="191"/>
+      <c r="H25" s="192"/>
       <c r="I25" t="s" s="203">
         <f>A25</f>
         <v>2500</v>
@@ -18247,17 +18239,17 @@
       <c r="A26" t="s" s="202">
         <v>2501</v>
       </c>
-      <c r="B26" s="192"/>
-      <c r="C26" s="192"/>
-      <c r="D26" t="s" s="191">
+      <c r="B26" s="190"/>
+      <c r="C26" s="190"/>
+      <c r="D26" t="s" s="189">
         <v>2502</v>
       </c>
-      <c r="E26" t="s" s="195">
+      <c r="E26" t="s" s="193">
         <v>2503</v>
       </c>
-      <c r="F26" s="193"/>
-      <c r="G26" s="193"/>
-      <c r="H26" s="194"/>
+      <c r="F26" s="191"/>
+      <c r="G26" s="191"/>
+      <c r="H26" s="192"/>
       <c r="I26" t="s" s="203">
         <f>A26</f>
         <v>2504</v>
@@ -18267,13 +18259,13 @@
       <c r="A27" t="s" s="202">
         <v>2505</v>
       </c>
-      <c r="B27" s="192"/>
-      <c r="C27" s="192"/>
-      <c r="D27" s="193"/>
-      <c r="E27" s="192"/>
-      <c r="F27" s="193"/>
-      <c r="G27" s="193"/>
-      <c r="H27" s="194"/>
+      <c r="B27" s="190"/>
+      <c r="C27" s="190"/>
+      <c r="D27" s="191"/>
+      <c r="E27" s="190"/>
+      <c r="F27" s="191"/>
+      <c r="G27" s="191"/>
+      <c r="H27" s="192"/>
       <c r="I27" t="s" s="203">
         <f>A27</f>
         <v>2506</v>
@@ -18283,13 +18275,13 @@
       <c r="A28" t="s" s="202">
         <v>2507</v>
       </c>
-      <c r="B28" s="192"/>
-      <c r="C28" s="192"/>
-      <c r="D28" s="193"/>
-      <c r="E28" s="192"/>
-      <c r="F28" s="193"/>
-      <c r="G28" s="193"/>
-      <c r="H28" s="194"/>
+      <c r="B28" s="190"/>
+      <c r="C28" s="190"/>
+      <c r="D28" s="191"/>
+      <c r="E28" s="190"/>
+      <c r="F28" s="191"/>
+      <c r="G28" s="191"/>
+      <c r="H28" s="192"/>
       <c r="I28" t="s" s="203">
         <f>A28</f>
         <v>2508</v>
@@ -18299,13 +18291,13 @@
       <c r="A29" t="s" s="202">
         <v>2509</v>
       </c>
-      <c r="B29" s="192"/>
-      <c r="C29" s="192"/>
-      <c r="D29" s="193"/>
-      <c r="E29" s="192"/>
-      <c r="F29" s="193"/>
-      <c r="G29" s="193"/>
-      <c r="H29" s="194"/>
+      <c r="B29" s="190"/>
+      <c r="C29" s="190"/>
+      <c r="D29" s="191"/>
+      <c r="E29" s="190"/>
+      <c r="F29" s="191"/>
+      <c r="G29" s="191"/>
+      <c r="H29" s="192"/>
       <c r="I29" t="s" s="203">
         <f>A29</f>
         <v>2510</v>
@@ -18315,13 +18307,13 @@
       <c r="A30" t="s" s="202">
         <v>2511</v>
       </c>
-      <c r="B30" s="192"/>
-      <c r="C30" s="192"/>
-      <c r="D30" s="193"/>
-      <c r="E30" s="192"/>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="194"/>
+      <c r="B30" s="190"/>
+      <c r="C30" s="190"/>
+      <c r="D30" s="191"/>
+      <c r="E30" s="190"/>
+      <c r="F30" s="191"/>
+      <c r="G30" s="191"/>
+      <c r="H30" s="192"/>
       <c r="I30" t="s" s="203">
         <f>A30</f>
         <v>2512</v>
@@ -18331,15 +18323,15 @@
       <c r="A31" t="s" s="202">
         <v>2513</v>
       </c>
-      <c r="B31" s="192"/>
-      <c r="C31" s="192"/>
-      <c r="D31" s="193"/>
+      <c r="B31" s="190"/>
+      <c r="C31" s="190"/>
+      <c r="D31" s="191"/>
       <c r="E31" t="s" s="120">
         <v>2514</v>
       </c>
-      <c r="F31" s="193"/>
-      <c r="G31" s="193"/>
-      <c r="H31" s="194"/>
+      <c r="F31" s="191"/>
+      <c r="G31" s="191"/>
+      <c r="H31" s="192"/>
       <c r="I31" t="s" s="203">
         <f>A31</f>
         <v>2515</v>
@@ -18349,13 +18341,13 @@
       <c r="A32" t="s" s="202">
         <v>2516</v>
       </c>
-      <c r="B32" s="192"/>
-      <c r="C32" s="192"/>
-      <c r="D32" s="193"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="193"/>
-      <c r="G32" s="193"/>
-      <c r="H32" s="194"/>
+      <c r="B32" s="190"/>
+      <c r="C32" s="190"/>
+      <c r="D32" s="191"/>
+      <c r="E32" s="190"/>
+      <c r="F32" s="191"/>
+      <c r="G32" s="191"/>
+      <c r="H32" s="192"/>
       <c r="I32" t="s" s="203">
         <f>A32</f>
         <v>2517</v>
@@ -18365,17 +18357,17 @@
       <c r="A33" t="s" s="202">
         <v>2518</v>
       </c>
-      <c r="B33" s="192"/>
-      <c r="C33" s="192"/>
-      <c r="D33" t="s" s="191">
+      <c r="B33" s="190"/>
+      <c r="C33" s="190"/>
+      <c r="D33" t="s" s="189">
         <v>2519</v>
       </c>
-      <c r="E33" t="s" s="195">
+      <c r="E33" t="s" s="193">
         <v>2520</v>
       </c>
-      <c r="F33" s="193"/>
-      <c r="G33" s="193"/>
-      <c r="H33" s="194"/>
+      <c r="F33" s="191"/>
+      <c r="G33" s="191"/>
+      <c r="H33" s="192"/>
       <c r="I33" t="s" s="203">
         <f>A33</f>
         <v>2521</v>
@@ -18385,17 +18377,17 @@
       <c r="A34" t="s" s="202">
         <v>2522</v>
       </c>
-      <c r="B34" s="192"/>
-      <c r="C34" s="192"/>
-      <c r="D34" t="s" s="191">
+      <c r="B34" s="190"/>
+      <c r="C34" s="190"/>
+      <c r="D34" t="s" s="189">
         <v>2519</v>
       </c>
-      <c r="E34" t="s" s="195">
+      <c r="E34" t="s" s="193">
         <v>2523</v>
       </c>
-      <c r="F34" s="193"/>
-      <c r="G34" s="193"/>
-      <c r="H34" s="194"/>
+      <c r="F34" s="191"/>
+      <c r="G34" s="191"/>
+      <c r="H34" s="192"/>
       <c r="I34" t="s" s="203">
         <f>A34</f>
         <v>2524</v>
@@ -18405,17 +18397,17 @@
       <c r="A35" t="s" s="202">
         <v>2525</v>
       </c>
-      <c r="B35" s="192"/>
-      <c r="C35" s="192"/>
-      <c r="D35" t="s" s="191">
+      <c r="B35" s="190"/>
+      <c r="C35" s="190"/>
+      <c r="D35" t="s" s="189">
         <v>2519</v>
       </c>
-      <c r="E35" t="s" s="195">
+      <c r="E35" t="s" s="193">
         <v>2526</v>
       </c>
-      <c r="F35" s="193"/>
-      <c r="G35" s="193"/>
-      <c r="H35" s="194"/>
+      <c r="F35" s="191"/>
+      <c r="G35" s="191"/>
+      <c r="H35" s="192"/>
       <c r="I35" t="s" s="203">
         <f>A35</f>
         <v>2527</v>
@@ -23688,9 +23680,7 @@
   </sheetPr>
   <dimension ref="A1:O166"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -23702,7 +23692,7 @@
     <col min="6" max="6" width="29.8516" style="112" customWidth="1"/>
     <col min="7" max="7" width="32" style="112" customWidth="1"/>
     <col min="8" max="13" width="16.3516" style="112" customWidth="1"/>
-    <col min="14" max="14" width="36.4141" style="112" customWidth="1"/>
+    <col min="14" max="14" width="36.5" style="112" customWidth="1"/>
     <col min="15" max="15" width="16.3516" style="112" customWidth="1"/>
     <col min="16" max="16384" width="16.3516" style="112" customWidth="1"/>
   </cols>
@@ -29666,7 +29656,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E148" r:id="rId1" location="" tooltip="" display="https://haveibeenpwned.com"/>
+    <hyperlink ref="E148" r:id="rId1" location="" tooltip="" display="Playbook 1: Create a standard reporting format and method for social platforms for reporting false accounts. &#10;Playbook 2: &#10;- Is the account compromised? &#10;- Is it known to be associated with threat actors &#10;- common/random name &#10;- Names violate terms of service &#10;- Dormant account &#10;- Change of country IP&#10;- Social network growth patterns (number of friends etc) &#10;- Evidence of linguistic artifacts (multiple fingerprints, terms/idiosyncrasies )&#10;- Community vs. narrative vs. individuals &#10;Playbook 3: Report suspected bots. &#10;- Report ToS violations. &#10;-  In all playbooks the platform must force user verification, credential reset and enable MFA. Suspend the account if it cannot be verified.&#10;Playbook 1: Use sites like https://haveibeenpwned.com to detect compromised and at risk user accounts. &#10;Playbook 2: Monitor for unusual account usage (use of VPN, new geographic location, unusual usage hours, etc). &#10;Playbook 3: Detect sudden deviation in user sentiment such as suddenly dropping hashtags linked to extremist content.&#10;Playbook 4: Purchase &quot;likes&quot;, &quot;retweets&quot; and other vehicles which identify a bot and/or hijacked account. Ban the account.&#10;Playbook 5: Detect hijacked account and spam their posts. &quot;OP is a known disinformation bot. http://link.to.proof[.]com&quot;"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
chg: add techniques for counters
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -3718,9 +3718,9 @@
 TA10 - Go Physical
 T0007 - Create fake Social Media Profiles / Pages / Groups
 T0009 - Create fake experts
+T0045 - Use fale experts
 T0011 - Hijack legitimate account
 T0014 - Create funding campaigns
-T0017 - Promote online funding
 T0018 - Paid targeted ads
 T0045 - Use fake experts</t>
   </si>
@@ -3738,9 +3738,7 @@
 TA09 - Exposure
 TA10 - Go Physical
 T0007 - Create fake Social Media Profiles / Pages / Groups
-T0011 - Hijack legitimate account
-T0017 - Promote online funding
-T0045 - Use fake experts</t>
+T0043 - Use SMS/ WhatsApp/ Chat apps</t>
   </si>
   <si>
     <t xml:space="preserve">C00136</t>
@@ -3754,12 +3752,28 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">TA08 - Pump Priming
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TA08 - Pump Priming
 TA09 - Exposure
 TA10 - Go Physical
-T0005 - Center of Gravity Analysis
 T0010 - Cultivate ignorant agents
-T0029 - Manipulate online polls</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0020 - Trial content
+T0063 - Social media engagement</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00137</t>
@@ -18909,8 +18923,8 @@
   </sheetPr>
   <dimension ref="A1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N100" activeCellId="0" sqref="N100"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N97" activeCellId="0" sqref="N97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="13.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22390,7 +22404,7 @@
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
       <c r="K97" s="52" t="s">
-        <v>605</v>
+        <v>441</v>
       </c>
       <c r="L97" s="52" t="s">
         <v>668</v>
@@ -22428,7 +22442,7 @@
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
       <c r="K98" s="52" t="s">
-        <v>605</v>
+        <v>477</v>
       </c>
       <c r="L98" s="52" t="s">
         <v>668</v>
@@ -22464,7 +22478,7 @@
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
       <c r="K99" s="52" t="s">
-        <v>605</v>
+        <v>558</v>
       </c>
       <c r="L99" s="52" t="s">
         <v>668</v>

</xml_diff>

<commit_message>
chg: update countermeasures C00056
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -3085,7 +3085,7 @@
     <t xml:space="preserve">C00056</t>
   </si>
   <si>
-    <t xml:space="preserve">Get off social media</t>
+    <t xml:space="preserve">Encourage people to leave social media</t>
   </si>
   <si>
     <t xml:space="preserve">We don't expect this to work</t>
@@ -19464,7 +19464,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N35" activeCellId="0" sqref="N35"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20747,7 +20747,7 @@
       <c r="N34" s="58"/>
       <c r="O34" s="24" t="str">
         <f aca="false">A34&amp;" - "&amp;B34</f>
-        <v>C00056 - Get off social media</v>
+        <v>C00056 - Encourage people to leave social media</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
chg: update countermeasures C00053
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -3077,9 +3077,7 @@
     <t xml:space="preserve">I00004</t>
   </si>
   <si>
-    <t xml:space="preserve">T0011 - Hijack accounts
-TA06 - Develop Content (D2 Deny)
-T0008 - Create fake or imposter news sites</t>
+    <t xml:space="preserve">T0011 - Hijack legitimate accounts</t>
   </si>
   <si>
     <t xml:space="preserve">C00056</t>
@@ -19464,7 +19462,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00048
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -3023,10 +3023,33 @@
     <t xml:space="preserve">Rand2237 and Dalton19</t>
   </si>
   <si>
-    <t xml:space="preserve">TA08 - Pump Priming
-T0048 - Cow online opinion leaders
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0010 - Cultivate ignorant agents
+T0045 - Use fake experts
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0048 - Cow online opinion leaders
+T0051 - Fabricate social media comment
+T0052 - Teriary sites amplify news
+T0053 - Twitter trolls amplify and manipulate
+T0054 - Twitter bots amplify
+T0056 - Dedicated channel disseminate information pollution
 T0057 - Organise remote rallies and events
+T0060 - Continue to amplify
 T0061 - Sell merchandising</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00051</t>
@@ -3073,7 +3096,24 @@
     <t xml:space="preserve">A004 - activist</t>
   </si>
   <si>
-    <t xml:space="preserve">T0012 - Use concealment</t>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0012 - Use concealment
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0030 - Backstop personas</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00053</t>
@@ -19486,8 +19526,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20615,7 +20655,7 @@
         <v>790</v>
       </c>
       <c r="M30" s="20"/>
-      <c r="N30" s="55" t="s">
+      <c r="N30" s="61" t="s">
         <v>847</v>
       </c>
       <c r="O30" s="24" t="str">
@@ -20691,7 +20731,7 @@
         <v>726</v>
       </c>
       <c r="M32" s="20"/>
-      <c r="N32" s="52" t="s">
+      <c r="N32" s="55" t="s">
         <v>857</v>
       </c>
       <c r="O32" s="24" t="str">

</xml_diff>

<commit_message>
chg: update countermeasures C00044
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2981,16 +2981,37 @@
     <t xml:space="preserve">Keep people from posting to social media immediately</t>
   </si>
   <si>
-    <t xml:space="preserve">My interpretation is that this is method would be used to slow down activities or force a small delay between posts or replies to new posts.</t>
+    <t xml:space="preserve">Platforms can introduce friction to slow down activities, force a small delay between posts, or replies to posts.</t>
   </si>
   <si>
     <t xml:space="preserve">Rate restrict via regulation posting above a statistical threshold
 Unless account is de-anonymized and advertised as automated messaging</t>
   </si>
   <si>
-    <t xml:space="preserve">TA07 - Channel Selection
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0029 - Manipulate online polls
 T0049 - Flooding
-T0054 - Twitter bots amplify</t>
+T0054 - Twitter bots amplify
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0053 - Twitter trolls amplify and manipulate
+T0055 - Use hashtag
+T0056 - Dedicated channel disseminate information pollution
+T0051 - Fabricate social media comment
+T0050 - Cheerleading domestic social media ops</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00046</t>
@@ -3001,7 +3022,7 @@
   <si>
     <t xml:space="preserve">T0010 - Cultivate ignorant agents
 T0044 - Seed distortions
-T0021 – Memes
+T0021 - Memes
 T0022 - Conspiracy narratives
 T0023 - Distort facts
 T0027 - Adapt existing narratives
@@ -3012,7 +3033,7 @@
 T0052 - Teriary sites amplify news
 T0053 - Twitter trolls amplify and manipulate
 T0054 - Twitter bots amplify
-T0056 - Dedicated channel disseminate information pollution
+T0056 – Dedicated channel disseminate information pollution
 T0057 - Organise remote rallies and events
 T0060 - Continue to amplify
 T0061 - Sell merchandising</t>
@@ -19554,7 +19575,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20544,7 +20565,7 @@
         <v>C00042 - Address truth contained in narratives</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="52.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="107.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
         <v>832</v>
       </c>
@@ -20586,7 +20607,7 @@
         <v>C00044 - Keep people from posting to social media immediately</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="202.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
         <v>837</v>
       </c>

</xml_diff>

<commit_message>
chg: update countermeasures C00042
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -19574,8 +19574,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20554,7 +20554,7 @@
         <v>441</v>
       </c>
       <c r="L26" s="52" t="s">
-        <v>668</v>
+        <v>726</v>
       </c>
       <c r="M26" s="20"/>
       <c r="N26" s="55" t="s">

</xml_diff>

<commit_message>
chg: update countermeasures C00040
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3883" uniqueCount="2061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3883" uniqueCount="2062">
   <si>
     <t xml:space="preserve">MASTER COPY OF AMITT TTPS</t>
   </si>
@@ -2955,7 +2955,9 @@
 - Academia ISAO</t>
   </si>
   <si>
-    <t xml:space="preserve">T0009 - Create fake experts</t>
+    <t xml:space="preserve">T0007 - Create fake social media profiles
+T0009 - Create fake experts
+T0012 - Use concealment</t>
   </si>
   <si>
     <t xml:space="preserve">C00042</t>
@@ -7439,6 +7441,9 @@
   </si>
   <si>
     <t xml:space="preserve">TA03 - Develop People</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0009 - Create fake experts</t>
   </si>
   <si>
     <t xml:space="preserve">Verify published research accreditation</t>
@@ -12702,10 +12707,10 @@
         <v>1987</v>
       </c>
       <c r="H3" s="79" t="s">
-        <v>828</v>
+        <v>1988</v>
       </c>
       <c r="I3" s="84" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="J3" s="82"/>
       <c r="K3" s="79" t="str">
@@ -12715,23 +12720,23 @@
     </row>
     <row r="4" customFormat="false" ht="200.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="79" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
       <c r="D4" s="83"/>
       <c r="E4" s="82"/>
       <c r="F4" s="80" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="G4" s="79" t="s">
         <v>1987</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>828</v>
+        <v>1988</v>
       </c>
       <c r="I4" s="84" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="J4" s="82"/>
       <c r="K4" s="79" t="str">
@@ -12741,17 +12746,17 @@
     </row>
     <row r="5" customFormat="false" ht="68.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="79" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B5" s="82"/>
       <c r="C5" s="82"/>
       <c r="D5" s="83"/>
       <c r="E5" s="82"/>
       <c r="F5" s="80" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="G5" s="79" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="H5" s="79" t="s">
         <v>661</v>
@@ -12876,7 +12881,7 @@
         <v>1976</v>
       </c>
       <c r="C1" s="77" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="D1" s="86"/>
       <c r="E1" s="85" t="s">
@@ -12893,15 +12898,15 @@
     </row>
     <row r="2" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="88" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
       <c r="D2" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E2" s="84" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="F2" s="83"/>
       <c r="G2" s="83"/>
@@ -12913,15 +12918,15 @@
     </row>
     <row r="3" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="88" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B3" s="82"/>
       <c r="C3" s="82"/>
       <c r="D3" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E3" s="84" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="F3" s="83"/>
       <c r="G3" s="83"/>
@@ -12933,12 +12938,12 @@
     </row>
     <row r="4" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="88" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
       <c r="D4" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E4" s="84" t="s">
         <v>5</v>
@@ -12953,15 +12958,15 @@
     </row>
     <row r="5" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="88" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B5" s="82"/>
       <c r="C5" s="82"/>
       <c r="D5" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E5" s="84" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="F5" s="83"/>
       <c r="G5" s="83"/>
@@ -12973,15 +12978,15 @@
     </row>
     <row r="6" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="88" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B6" s="82"/>
       <c r="C6" s="82"/>
       <c r="D6" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E6" s="84" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F6" s="83"/>
       <c r="G6" s="83"/>
@@ -12993,15 +12998,15 @@
     </row>
     <row r="7" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="88" t="s">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B7" s="82"/>
       <c r="C7" s="82"/>
       <c r="D7" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E7" s="84" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="F7" s="83"/>
       <c r="G7" s="83"/>
@@ -13013,15 +13018,15 @@
     </row>
     <row r="8" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="88" t="s">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B8" s="82"/>
       <c r="C8" s="82"/>
       <c r="D8" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F8" s="83"/>
       <c r="G8" s="83"/>
@@ -13033,20 +13038,20 @@
     </row>
     <row r="9" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="88" t="s">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B9" s="82"/>
       <c r="C9" s="82"/>
       <c r="D9" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E9" s="84" t="s">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="F9" s="83"/>
       <c r="G9" s="83"/>
       <c r="H9" s="80" t="s">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="I9" s="88" t="str">
         <f aca="false">A9</f>
@@ -13055,15 +13060,15 @@
     </row>
     <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="88" t="s">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B10" s="82"/>
       <c r="C10" s="82"/>
       <c r="D10" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E10" s="84" t="s">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="F10" s="83"/>
       <c r="G10" s="83"/>
@@ -13075,20 +13080,20 @@
     </row>
     <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="88" t="s">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B11" s="82"/>
       <c r="C11" s="82"/>
       <c r="D11" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E11" s="84" t="s">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="F11" s="83"/>
       <c r="G11" s="83"/>
       <c r="H11" s="80" t="s">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="I11" s="88" t="str">
         <f aca="false">A11</f>
@@ -13097,20 +13102,20 @@
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="88" t="s">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B12" s="82"/>
       <c r="C12" s="82"/>
       <c r="D12" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E12" s="84" t="s">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F12" s="83"/>
       <c r="G12" s="83"/>
       <c r="H12" s="80" t="s">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="I12" s="88" t="str">
         <f aca="false">A12</f>
@@ -13119,15 +13124,15 @@
     </row>
     <row r="13" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="88" t="s">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B13" s="82"/>
       <c r="C13" s="82"/>
       <c r="D13" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E13" s="84" t="s">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F13" s="83"/>
       <c r="G13" s="83"/>
@@ -13139,15 +13144,15 @@
     </row>
     <row r="14" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="88" t="s">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B14" s="82"/>
       <c r="C14" s="82"/>
       <c r="D14" s="79" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="E14" s="84" t="s">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="F14" s="83"/>
       <c r="G14" s="83"/>
@@ -13159,7 +13164,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="88" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B15" s="82"/>
       <c r="C15" s="82"/>
@@ -13175,13 +13180,13 @@
     </row>
     <row r="16" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="88" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B16" s="82"/>
       <c r="C16" s="82"/>
       <c r="D16" s="83"/>
       <c r="E16" s="54" t="s">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="F16" s="83"/>
       <c r="G16" s="83"/>
@@ -13193,13 +13198,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="88" t="s">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B17" s="82"/>
       <c r="C17" s="82"/>
       <c r="D17" s="83"/>
       <c r="E17" s="84" t="s">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="F17" s="83"/>
       <c r="G17" s="83"/>
@@ -13211,15 +13216,15 @@
     </row>
     <row r="18" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="88" t="s">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B18" s="82"/>
       <c r="C18" s="82"/>
       <c r="D18" s="79" t="s">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="E18" s="84" t="s">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="F18" s="83"/>
       <c r="G18" s="83"/>
@@ -13231,15 +13236,15 @@
     </row>
     <row r="19" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="88" t="s">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B19" s="82"/>
       <c r="C19" s="82"/>
       <c r="D19" s="79" t="s">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="F19" s="83"/>
       <c r="G19" s="83"/>
@@ -13251,7 +13256,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="88" t="s">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B20" s="82"/>
       <c r="C20" s="82"/>
@@ -13267,15 +13272,15 @@
     </row>
     <row r="21" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="88" t="s">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B21" s="82"/>
       <c r="C21" s="82"/>
       <c r="D21" s="79" t="s">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="E21" s="84" t="s">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="F21" s="83"/>
       <c r="G21" s="83"/>
@@ -13287,15 +13292,15 @@
     </row>
     <row r="22" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="88" t="s">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B22" s="82"/>
       <c r="C22" s="82"/>
       <c r="D22" s="79" t="s">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="E22" s="84" t="s">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="F22" s="83"/>
       <c r="G22" s="83"/>
@@ -13307,7 +13312,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="88" t="s">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B23" s="82"/>
       <c r="C23" s="82"/>
@@ -13323,7 +13328,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="88" t="s">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B24" s="82"/>
       <c r="C24" s="82"/>
@@ -13339,7 +13344,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="88" t="s">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B25" s="82"/>
       <c r="C25" s="82"/>
@@ -13355,15 +13360,15 @@
     </row>
     <row r="26" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="88" t="s">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B26" s="82"/>
       <c r="C26" s="82"/>
       <c r="D26" s="79" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="E26" s="84" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="F26" s="83"/>
       <c r="G26" s="83"/>
@@ -13375,7 +13380,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="88" t="s">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B27" s="82"/>
       <c r="C27" s="82"/>
@@ -13391,7 +13396,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="88" t="s">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B28" s="82"/>
       <c r="C28" s="82"/>
@@ -13407,7 +13412,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="88" t="s">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B29" s="82"/>
       <c r="C29" s="82"/>
@@ -13423,7 +13428,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="88" t="s">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B30" s="82"/>
       <c r="C30" s="82"/>
@@ -13439,13 +13444,13 @@
     </row>
     <row r="31" customFormat="false" ht="35.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="88" t="s">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B31" s="82"/>
       <c r="C31" s="82"/>
       <c r="D31" s="83"/>
       <c r="E31" s="54" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="F31" s="83"/>
       <c r="G31" s="83"/>
@@ -13457,7 +13462,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="88" t="s">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B32" s="82"/>
       <c r="C32" s="82"/>
@@ -13473,15 +13478,15 @@
     </row>
     <row r="33" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="88" t="s">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B33" s="82"/>
       <c r="C33" s="82"/>
       <c r="D33" s="79" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="E33" s="84" t="s">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="F33" s="83"/>
       <c r="G33" s="83"/>
@@ -13493,15 +13498,15 @@
     </row>
     <row r="34" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="88" t="s">
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="B34" s="82"/>
       <c r="C34" s="82"/>
       <c r="D34" s="79" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="E34" s="84" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="F34" s="83"/>
       <c r="G34" s="83"/>
@@ -13513,15 +13518,15 @@
     </row>
     <row r="35" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="88" t="s">
-        <v>2059</v>
+        <v>2060</v>
       </c>
       <c r="B35" s="82"/>
       <c r="C35" s="82"/>
       <c r="D35" s="79" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="E35" s="84" t="s">
-        <v>2060</v>
+        <v>2061</v>
       </c>
       <c r="F35" s="83"/>
       <c r="G35" s="83"/>
@@ -19575,7 +19580,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20523,7 +20528,7 @@
         <v>712</v>
       </c>
       <c r="M25" s="20"/>
-      <c r="N25" s="52" t="s">
+      <c r="N25" s="55" t="s">
         <v>828</v>
       </c>
       <c r="O25" s="24" t="str">

</xml_diff>

<commit_message>
chg: update countermeasures C00036
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2933,12 +2933,39 @@
 -Publicize this by targeting their in-group competitors (ignorant agents)</t>
   </si>
   <si>
-    <t xml:space="preserve">T0005 - Center of Gravity Analysis
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0005 - Center of Gravity Analysis
 T0007 - Create fake Social Media Profiles / Pages / Groups
-T0017 - Promote online funding
-T0025 - Leak altered documents
-T0056 - Dedicated channels disseminate information pollution
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0010 - Cultivate ignorant agents
+T0012 - Use concealment
+T0030 - Backstop personas
+T0045 - Use fake experts
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0056 - Dedicated channels disseminate information pollution
 T0057 - Organise remote rallies and events</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00040</t>
@@ -19580,7 +19607,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00032
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3884" uniqueCount="2063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3885" uniqueCount="2063">
   <si>
     <t xml:space="preserve">MASTER COPY OF AMITT TTPS</t>
   </si>
@@ -2907,6 +2907,9 @@
 Playbook 2: Hijack (man in the middle) redirect from bad content to good content</t>
   </si>
   <si>
+    <t xml:space="preserve">T0055 - Use hashtag</t>
+  </si>
+  <si>
     <t xml:space="preserve">C00034</t>
   </si>
   <si>
@@ -3922,9 +3925,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hashtag jacking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T0055 - Use hashtag</t>
   </si>
   <si>
     <t xml:space="preserve">C00101</t>
@@ -19609,7 +19609,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20449,7 +20449,9 @@
         <v>668</v>
       </c>
       <c r="M22" s="20"/>
-      <c r="N22" s="58"/>
+      <c r="N22" s="58" t="s">
+        <v>815</v>
+      </c>
       <c r="O22" s="24" t="str">
         <f aca="false">A22&amp;" - "&amp;B22</f>
         <v>C00032 - Hijack content and link to truth- based info</v>
@@ -20457,16 +20459,16 @@
     </row>
     <row r="23" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>706</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
@@ -20484,7 +20486,7 @@
       </c>
       <c r="M23" s="20"/>
       <c r="N23" s="60" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="O23" s="24" t="str">
         <f aca="false">A23&amp;" - "&amp;B23</f>
@@ -20493,19 +20495,19 @@
     </row>
     <row r="24" customFormat="false" ht="152.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -20522,7 +20524,7 @@
       </c>
       <c r="M24" s="20"/>
       <c r="N24" s="55" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="O24" s="24" t="str">
         <f aca="false">A24&amp;" - "&amp;B24</f>
@@ -20531,19 +20533,19 @@
     </row>
     <row r="25" customFormat="false" ht="50.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>794</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -20560,7 +20562,7 @@
       </c>
       <c r="M25" s="20"/>
       <c r="N25" s="55" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="O25" s="24" t="str">
         <f aca="false">A25&amp;" - "&amp;B25</f>
@@ -20569,10 +20571,10 @@
     </row>
     <row r="26" customFormat="false" ht="182.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>765</v>
@@ -20594,7 +20596,7 @@
       </c>
       <c r="M26" s="20"/>
       <c r="N26" s="55" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="O26" s="24" t="str">
         <f aca="false">A26&amp;" - "&amp;B26</f>
@@ -20603,19 +20605,19 @@
     </row>
     <row r="27" customFormat="false" ht="107.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>706</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>761</v>
@@ -20636,7 +20638,7 @@
       </c>
       <c r="M27" s="20"/>
       <c r="N27" s="55" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="O27" s="24" t="str">
         <f aca="false">A27&amp;" - "&amp;B27</f>
@@ -20645,13 +20647,13 @@
     </row>
     <row r="28" customFormat="false" ht="202.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="20"/>
@@ -20670,7 +20672,7 @@
       </c>
       <c r="M28" s="20"/>
       <c r="N28" s="60" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="O28" s="24" t="str">
         <f aca="false">A28&amp;" - "&amp;B28</f>
@@ -20679,13 +20681,13 @@
     </row>
     <row r="29" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -20704,7 +20706,7 @@
       </c>
       <c r="M29" s="20"/>
       <c r="N29" s="56" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="O29" s="24" t="str">
         <f aca="false">A29&amp;" - "&amp;B29</f>
@@ -20713,19 +20715,19 @@
     </row>
     <row r="30" customFormat="false" ht="352.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>710</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
@@ -20733,7 +20735,7 @@
         <v>749</v>
       </c>
       <c r="I30" s="61" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="52" t="s">
@@ -20744,7 +20746,7 @@
       </c>
       <c r="M30" s="20"/>
       <c r="N30" s="62" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="O30" s="24" t="str">
         <f aca="false">A30&amp;" - "&amp;B30</f>
@@ -20753,20 +20755,20 @@
     </row>
     <row r="31" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>730</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="24" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="G31" s="24"/>
       <c r="H31" s="24" t="s">
@@ -20782,7 +20784,7 @@
       </c>
       <c r="M31" s="20"/>
       <c r="N31" s="62" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="O31" s="24" t="str">
         <f aca="false">A31&amp;" - "&amp;B31</f>
@@ -20791,20 +20793,20 @@
     </row>
     <row r="32" customFormat="false" ht="26.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="24" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="24" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="24" t="s">
@@ -20820,7 +20822,7 @@
       </c>
       <c r="M32" s="20"/>
       <c r="N32" s="55" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="O32" s="24" t="str">
         <f aca="false">A32&amp;" - "&amp;B32</f>
@@ -20829,28 +20831,28 @@
     </row>
     <row r="33" customFormat="false" ht="134.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="24" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="24" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="24" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="24" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="K33" s="52" t="s">
         <v>477</v>
@@ -20860,7 +20862,7 @@
       </c>
       <c r="M33" s="20"/>
       <c r="N33" s="55" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="O33" s="24" t="str">
         <f aca="false">A33&amp;" - "&amp;B33</f>
@@ -20869,16 +20871,16 @@
     </row>
     <row r="34" customFormat="false" ht="26.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="24" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>706</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -20903,16 +20905,16 @@
     </row>
     <row r="35" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="24" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>759</v>
       </c>
       <c r="D35" s="54" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
@@ -20930,7 +20932,7 @@
       </c>
       <c r="M35" s="20"/>
       <c r="N35" s="55" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="O35" s="24" t="str">
         <f aca="false">A35&amp;" - "&amp;B35</f>
@@ -20939,10 +20941,10 @@
     </row>
     <row r="36" customFormat="false" ht="62.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="24" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>794</v>
@@ -20964,7 +20966,7 @@
       </c>
       <c r="M36" s="20"/>
       <c r="N36" s="60" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="O36" s="24" t="str">
         <f aca="false">A36&amp;" - "&amp;B36</f>
@@ -20973,13 +20975,13 @@
     </row>
     <row r="37" customFormat="false" ht="74.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="24" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
@@ -21000,7 +21002,7 @@
       </c>
       <c r="M37" s="20"/>
       <c r="N37" s="55" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="O37" s="24" t="str">
         <f aca="false">A37&amp;" - "&amp;B37</f>
@@ -21009,16 +21011,16 @@
     </row>
     <row r="38" customFormat="false" ht="62.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="24" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>765</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="20"/>
@@ -21045,16 +21047,16 @@
     </row>
     <row r="39" customFormat="false" ht="26.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="24" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>759</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="24" t="s">
@@ -21074,7 +21076,7 @@
       </c>
       <c r="M39" s="20"/>
       <c r="N39" s="52" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="O39" s="24" t="str">
         <f aca="false">A39&amp;" - "&amp;B39</f>
@@ -21083,10 +21085,10 @@
     </row>
     <row r="40" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="24" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>806</v>
@@ -21108,7 +21110,7 @@
       </c>
       <c r="M40" s="20"/>
       <c r="N40" s="55" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="O40" s="24" t="str">
         <f aca="false">A40&amp;" - "&amp;B40</f>
@@ -21117,13 +21119,13 @@
     </row>
     <row r="41" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="24" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
@@ -21142,7 +21144,7 @@
       </c>
       <c r="M41" s="20"/>
       <c r="N41" s="55" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="O41" s="24" t="str">
         <f aca="false">A41&amp;" - "&amp;B41</f>
@@ -21151,16 +21153,16 @@
     </row>
     <row r="42" customFormat="false" ht="202.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="24" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>759</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
@@ -21178,7 +21180,7 @@
       </c>
       <c r="M42" s="20"/>
       <c r="N42" s="55" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="O42" s="24" t="str">
         <f aca="false">A42&amp;" - "&amp;B42</f>
@@ -21187,10 +21189,10 @@
     </row>
     <row r="43" customFormat="false" ht="52.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="24" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>759</v>
@@ -21212,7 +21214,7 @@
       </c>
       <c r="M43" s="20"/>
       <c r="N43" s="55" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="O43" s="24" t="str">
         <f aca="false">A43&amp;" - "&amp;B43</f>
@@ -21221,10 +21223,10 @@
     </row>
     <row r="44" customFormat="false" ht="143" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="24" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C44" s="24" t="s">
         <v>759</v>
@@ -21246,7 +21248,7 @@
       </c>
       <c r="M44" s="20"/>
       <c r="N44" s="55" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="O44" s="24" t="str">
         <f aca="false">A44&amp;" - "&amp;B44</f>
@@ -21255,24 +21257,24 @@
     </row>
     <row r="45" customFormat="false" ht="268.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="24" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>730</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="24" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="G45" s="24"/>
       <c r="H45" s="24" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="I45" s="59" t="s">
         <v>624</v>
@@ -21286,7 +21288,7 @@
       </c>
       <c r="M45" s="20"/>
       <c r="N45" s="55" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="O45" s="24" t="str">
         <f aca="false">A45&amp;" - "&amp;B45</f>
@@ -21295,22 +21297,22 @@
     </row>
     <row r="46" customFormat="false" ht="230.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="24" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="G46" s="24"/>
       <c r="H46" s="24" t="s">
@@ -21326,7 +21328,7 @@
       </c>
       <c r="M46" s="20"/>
       <c r="N46" s="55" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="O46" s="24" t="str">
         <f aca="false">A46&amp;" - "&amp;B46</f>
@@ -21335,10 +21337,10 @@
     </row>
     <row r="47" customFormat="false" ht="26.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="24" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>765</v>
@@ -21367,10 +21369,10 @@
     </row>
     <row r="48" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="24" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>759</v>
@@ -21392,7 +21394,7 @@
       </c>
       <c r="M48" s="20"/>
       <c r="N48" s="55" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="O48" s="24" t="str">
         <f aca="false">A48&amp;" - "&amp;B48</f>
@@ -21401,13 +21403,13 @@
     </row>
     <row r="49" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="24" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -21433,16 +21435,16 @@
     </row>
     <row r="50" customFormat="false" ht="110.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="24" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C50" s="24" t="s">
         <v>799</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -21460,7 +21462,7 @@
       </c>
       <c r="M50" s="20"/>
       <c r="N50" s="55" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="O50" s="24" t="str">
         <f aca="false">A50&amp;" - "&amp;B50</f>
@@ -21469,16 +21471,16 @@
     </row>
     <row r="51" customFormat="false" ht="188.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="24" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>799</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
@@ -21496,7 +21498,7 @@
       </c>
       <c r="M51" s="20"/>
       <c r="N51" s="55" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="O51" s="24" t="str">
         <f aca="false">A51&amp;" - "&amp;B51</f>
@@ -21505,16 +21507,16 @@
     </row>
     <row r="52" customFormat="false" ht="122.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="24" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C52" s="24" t="s">
         <v>710</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
@@ -21532,7 +21534,7 @@
       </c>
       <c r="M52" s="20"/>
       <c r="N52" s="56" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="O52" s="24" t="str">
         <f aca="false">A52&amp;" - "&amp;B52</f>
@@ -21541,16 +21543,16 @@
     </row>
     <row r="53" customFormat="false" ht="172.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="24" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>765</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
@@ -21568,7 +21570,7 @@
       </c>
       <c r="M53" s="20"/>
       <c r="N53" s="56" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="O53" s="24" t="str">
         <f aca="false">A53&amp;" - "&amp;B53</f>
@@ -21577,16 +21579,16 @@
     </row>
     <row r="54" customFormat="false" ht="118.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="24" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>799</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E54" s="20"/>
       <c r="F54" s="20"/>
@@ -21604,7 +21606,7 @@
       </c>
       <c r="M54" s="20"/>
       <c r="N54" s="55" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="O54" s="24" t="str">
         <f aca="false">A54&amp;" - "&amp;B54</f>
@@ -21613,16 +21615,16 @@
     </row>
     <row r="55" customFormat="false" ht="303.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="24" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C55" s="24" t="s">
         <v>710</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -21640,7 +21642,7 @@
       </c>
       <c r="M55" s="20"/>
       <c r="N55" s="63" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="O55" s="24" t="str">
         <f aca="false">A55&amp;" - "&amp;B55</f>
@@ -21649,16 +21651,16 @@
     </row>
     <row r="56" customFormat="false" ht="134.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="24" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>799</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E56" s="20"/>
       <c r="F56" s="20"/>
@@ -21676,7 +21678,7 @@
       </c>
       <c r="M56" s="20"/>
       <c r="N56" s="64" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="O56" s="24" t="str">
         <f aca="false">A56&amp;" - "&amp;B56</f>
@@ -21685,16 +21687,16 @@
     </row>
     <row r="57" customFormat="false" ht="172.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="24" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>806</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
@@ -21712,7 +21714,7 @@
       </c>
       <c r="M57" s="20"/>
       <c r="N57" s="64" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="O57" s="24" t="str">
         <f aca="false">A57&amp;" - "&amp;B57</f>
@@ -21721,10 +21723,10 @@
     </row>
     <row r="58" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="24" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>799</v>
@@ -21746,7 +21748,7 @@
       </c>
       <c r="M58" s="20"/>
       <c r="N58" s="55" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="O58" s="24" t="str">
         <f aca="false">A58&amp;" - "&amp;B58</f>
@@ -21755,16 +21757,16 @@
     </row>
     <row r="59" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="24" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>799</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="20"/>
@@ -21782,7 +21784,7 @@
       </c>
       <c r="M59" s="20"/>
       <c r="N59" s="55" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="O59" s="24" t="str">
         <f aca="false">A59&amp;" - "&amp;B59</f>
@@ -21791,23 +21793,23 @@
     </row>
     <row r="60" customFormat="false" ht="172.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="24" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>721</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="24" t="s">
         <v>618</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="H60" s="24" t="s">
         <v>413</v>
@@ -21822,7 +21824,7 @@
       </c>
       <c r="M60" s="20"/>
       <c r="N60" s="55" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="O60" s="24" t="str">
         <f aca="false">A60&amp;" - "&amp;B60</f>
@@ -21831,16 +21833,16 @@
     </row>
     <row r="61" customFormat="false" ht="152.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="24" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C61" s="24" t="s">
         <v>730</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="20"/>
@@ -21858,7 +21860,7 @@
       </c>
       <c r="M61" s="20"/>
       <c r="N61" s="55" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="O61" s="24" t="str">
         <f aca="false">A61&amp;" - "&amp;B61</f>
@@ -21867,16 +21869,16 @@
     </row>
     <row r="62" customFormat="false" ht="50.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="24" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C62" s="24" t="s">
         <v>710</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
@@ -21894,7 +21896,7 @@
       </c>
       <c r="M62" s="20"/>
       <c r="N62" s="52" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="O62" s="24" t="str">
         <f aca="false">A62&amp;" - "&amp;B62</f>
@@ -21903,10 +21905,10 @@
     </row>
     <row r="63" customFormat="false" ht="70.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="24" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>721</v>
@@ -21928,7 +21930,7 @@
       </c>
       <c r="M63" s="20"/>
       <c r="N63" s="55" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="O63" s="24" t="str">
         <f aca="false">A63&amp;" - "&amp;B63</f>
@@ -21937,10 +21939,10 @@
     </row>
     <row r="64" customFormat="false" ht="80.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="24" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C64" s="24" t="s">
         <v>706</v>
@@ -21966,7 +21968,7 @@
       </c>
       <c r="M64" s="20"/>
       <c r="N64" s="55" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="O64" s="24" t="str">
         <f aca="false">A64&amp;" - "&amp;B64</f>
@@ -21975,17 +21977,17 @@
     </row>
     <row r="65" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="24" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>706</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="24" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F65" s="24" t="s">
         <v>761</v>
@@ -22004,7 +22006,7 @@
       </c>
       <c r="M65" s="20"/>
       <c r="N65" s="55" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="O65" s="24" t="str">
         <f aca="false">A65&amp;" - "&amp;B65</f>
@@ -22013,10 +22015,10 @@
     </row>
     <row r="66" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="24" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B66" s="54" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>706</v>
@@ -22042,7 +22044,7 @@
       </c>
       <c r="M66" s="20"/>
       <c r="N66" s="55" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="O66" s="24" t="str">
         <f aca="false">A66&amp;" - "&amp;B66</f>
@@ -22051,10 +22053,10 @@
     </row>
     <row r="67" customFormat="false" ht="26.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="24" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C67" s="24" t="s">
         <v>799</v>
@@ -22076,7 +22078,7 @@
       </c>
       <c r="M67" s="20"/>
       <c r="N67" s="52" t="s">
-        <v>989</v>
+        <v>815</v>
       </c>
       <c r="O67" s="24" t="str">
         <f aca="false">A67&amp;" - "&amp;B67</f>
@@ -23197,7 +23199,7 @@
         <v>1103</v>
       </c>
       <c r="C99" s="24" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D99" s="24" t="s">
         <v>1104</v>
@@ -23275,7 +23277,7 @@
         <v>1113</v>
       </c>
       <c r="C101" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D101" s="24" t="s">
         <v>1114</v>
@@ -23387,7 +23389,7 @@
         <v>1125</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D104" s="24" t="s">
         <v>1126</v>
@@ -23429,7 +23431,7 @@
         <v>1130</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="D105" s="20" t="s">
         <v>1131</v>
@@ -23467,7 +23469,7 @@
         <v>1135</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D106" s="54" t="s">
         <v>1136</v>
@@ -23737,7 +23739,7 @@
         <v>1165</v>
       </c>
       <c r="C113" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D113" s="24" t="s">
         <v>1166</v>
@@ -23775,7 +23777,7 @@
         <v>1169</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D114" s="24" t="s">
         <v>1170</v>
@@ -24519,7 +24521,7 @@
         <v>1261</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="D133" s="24" t="s">
         <v>1262</v>
@@ -24570,7 +24572,7 @@
       </c>
       <c r="I134" s="20"/>
       <c r="J134" s="24" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="K134" s="55" t="s">
         <v>574</v>
@@ -25030,7 +25032,7 @@
     </row>
     <row r="5" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>1318</v>

</xml_diff>

<commit_message>
chg: update countermeasures C00031
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2889,9 +2889,27 @@
     <t xml:space="preserve">CAVEAT: some element of disinformation is simply filling the information space with so much data that it overwhelms people and they shutdown. Any swarm-counter-narrative needs to be cautious of this outcome.</t>
   </si>
   <si>
-    <t xml:space="preserve">T0002 - Facilitate State Propaganda
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0002 - Facilitate State Propaganda
 T0003 - Leverage Existing Narratives
-T0006 - Create Master Narratives</t>
+T0006 - Create Master Narratives
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0027 - Adapt existing narratives
+T0028 - Create competing narratives</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00032</t>
@@ -19608,8 +19626,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00029
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="2064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3887" uniqueCount="2064">
   <si>
     <t xml:space="preserve">MASTER COPY OF AMITT TTPS</t>
   </si>
@@ -2860,22 +2860,22 @@
 -Obtain real-life identity of ignorant agents, to further disrupt their influence activities</t>
   </si>
   <si>
-    <t xml:space="preserve">C00030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Develop a compelling counter narrative (truth based)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example: Reality Team.
-https://www.isdglobal.org/wp-content/uploads/2016/06/Counter-narrative-Handbook_1.pdf </t>
-  </si>
-  <si>
     <t xml:space="preserve">T0002 - Facilitate State Propaganda
 T0003 - Leverage Existing Narratives
 T0006 - Create Master Narratives
 T0027 - Adapt existing narratives
 T0028 - Create competing narratives
 T0022 - Conspiracy narratives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C00030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Develop a compelling counter narrative (truth based)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example: Reality Team.
+https://www.isdglobal.org/wp-content/uploads/2016/06/Counter-narrative-Handbook_1.pdf </t>
   </si>
   <si>
     <t xml:space="preserve">C00031</t>
@@ -8387,7 +8387,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="N19 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8892,7 +8892,7 @@
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11180,7 +11180,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11351,7 +11351,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11619,7 +11619,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12318,7 +12318,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12504,7 +12504,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12682,7 +12682,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12920,7 +12920,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13620,7 +13620,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13776,7 +13776,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14081,7 +14081,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15279,7 +15279,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15920,7 +15920,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16479,7 +16479,7 @@
   <dimension ref="A1:O95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="topLeft" activeCell="A95" activeCellId="1" sqref="N19 A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19635,7 +19635,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20365,7 +20365,9 @@
         <v>668</v>
       </c>
       <c r="M19" s="20"/>
-      <c r="N19" s="58"/>
+      <c r="N19" s="60" t="s">
+        <v>801</v>
+      </c>
       <c r="O19" s="24" t="str">
         <f aca="false">A19&amp;" - "&amp;B19</f>
         <v>C00029 - Create fake website to issue counter narrative and counter narrative through physical merchandise</v>
@@ -20373,16 +20375,16 @@
     </row>
     <row r="20" customFormat="false" ht="102.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C20" s="24" t="s">
         <v>799</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -20400,7 +20402,7 @@
       </c>
       <c r="M20" s="20"/>
       <c r="N20" s="60" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="O20" s="24" t="str">
         <f aca="false">A20&amp;" - "&amp;B20</f>
@@ -24900,7 +24902,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00027
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2815,15 +2815,35 @@
     <t xml:space="preserve">D7 Deter</t>
   </si>
   <si>
-    <t xml:space="preserve">TA01 - Strategic Planning
-TA08 - Pump Priming
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
+T0002 - Facilitate State Propaganda
+T0003 - Leverage Existing Narratives
 T0006 - Create Master Narratives
+T0027 - Adapt existing narratives
+T0028 - Create competing narratives
 T0022 - Conspiracy narratives
-T0023 - Distort facts
-T0027 - Adapt existing narratives
-T0047 - Muzzle social media as a political force
+T0021 - Memes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0023 - Distort facts
 T0048 - Cow online opinion leaders
-T0053 - Twitter trolls amplify and manipulate</t>
+T0053 - Twitter trolls amplify and manipulate
+T0044 - Seed distortions
+T0039 - Bait legitimate influencers</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00028</t>
@@ -8251,16 +8271,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8387,7 +8407,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="N19 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8892,7 +8912,7 @@
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11180,7 +11200,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11351,7 +11371,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11619,7 +11639,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12318,7 +12338,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12504,7 +12524,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12682,7 +12702,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12920,7 +12940,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13620,7 +13640,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13776,7 +13796,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14081,7 +14101,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15279,7 +15299,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15920,7 +15940,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16479,7 +16499,7 @@
   <dimension ref="A1:O95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="1" sqref="N19 A95"/>
+      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19634,8 +19654,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20293,7 +20313,7 @@
         <v>790</v>
       </c>
       <c r="M17" s="20"/>
-      <c r="N17" s="55" t="s">
+      <c r="N17" s="60" t="s">
         <v>791</v>
       </c>
       <c r="O17" s="24" t="str">
@@ -20365,7 +20385,7 @@
         <v>668</v>
       </c>
       <c r="M19" s="20"/>
-      <c r="N19" s="60" t="s">
+      <c r="N19" s="61" t="s">
         <v>801</v>
       </c>
       <c r="O19" s="24" t="str">
@@ -20401,7 +20421,7 @@
         <v>668</v>
       </c>
       <c r="M20" s="20"/>
-      <c r="N20" s="60" t="s">
+      <c r="N20" s="61" t="s">
         <v>801</v>
       </c>
       <c r="O20" s="24" t="str">
@@ -20515,7 +20535,7 @@
         <v>726</v>
       </c>
       <c r="M23" s="20"/>
-      <c r="N23" s="60" t="s">
+      <c r="N23" s="61" t="s">
         <v>820</v>
       </c>
       <c r="O23" s="24" t="str">
@@ -20701,7 +20721,7 @@
         <v>726</v>
       </c>
       <c r="M28" s="20"/>
-      <c r="N28" s="60" t="s">
+      <c r="N28" s="61" t="s">
         <v>842</v>
       </c>
       <c r="O28" s="24" t="str">
@@ -20764,7 +20784,7 @@
       <c r="H30" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="I30" s="61" t="s">
+      <c r="I30" s="62" t="s">
         <v>851</v>
       </c>
       <c r="J30" s="4"/>
@@ -20775,7 +20795,7 @@
         <v>790</v>
       </c>
       <c r="M30" s="20"/>
-      <c r="N30" s="62" t="s">
+      <c r="N30" s="60" t="s">
         <v>852</v>
       </c>
       <c r="O30" s="24" t="str">
@@ -20813,7 +20833,7 @@
         <v>712</v>
       </c>
       <c r="M31" s="20"/>
-      <c r="N31" s="62" t="s">
+      <c r="N31" s="60" t="s">
         <v>857</v>
       </c>
       <c r="O31" s="24" t="str">
@@ -20995,7 +21015,7 @@
         <v>712</v>
       </c>
       <c r="M36" s="20"/>
-      <c r="N36" s="60" t="s">
+      <c r="N36" s="61" t="s">
         <v>880</v>
       </c>
       <c r="O36" s="24" t="str">
@@ -24902,7 +24922,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00024
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2781,11 +2781,17 @@
     <t xml:space="preserve">Includes promoting constructive narratives i.e. not polarising (e.g. pro-life, pro-choice, pro-USA).  Includes promoting identity neutral narratives. </t>
   </si>
   <si>
-    <t xml:space="preserve">TA01 - Strategic Planning
+    <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
+T0002 - Facilitate State Propaganda
+T0003 - Leverage Existing Narratives
 T0006 - Create Master Narratives
 T0027 - Adapt existing narratives
+T0028 - Create competing narratives
 T0022 - Conspiracy narratives
-T0023 - Distort facts</t>
+T0023 - Distort facts
+T0053 - Twitter trolls amplify and manipulate
+T0044 - Seed distortions
+</t>
   </si>
   <si>
     <t xml:space="preserve">C00026</t>
@@ -19659,7 +19665,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20241,7 +20247,7 @@
         <v>726</v>
       </c>
       <c r="M15" s="20"/>
-      <c r="N15" s="55" t="s">
+      <c r="N15" s="60" t="s">
         <v>782</v>
       </c>
       <c r="O15" s="24" t="str">

</xml_diff>

<commit_message>
chg: update countermeasures C00021
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2760,15 +2760,6 @@
     <t xml:space="preserve">Encourage in-person communication</t>
   </si>
   <si>
-    <t xml:space="preserve">C00022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Innoculate. Positive campaign to promote feeling of safety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used to counter ability based and fear based attacks</t>
-  </si>
-  <si>
     <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
 T0002 - Facilitate State Propaganda
 T0003 - Leverage Existing Narratives
@@ -2780,6 +2771,15 @@
 T0053 - Twitter trolls amplify and manipulate
 T0044 - Seed distortions
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C00022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Innoculate. Positive campaign to promote feeling of safety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to counter ability based and fear based attacks</t>
   </si>
   <si>
     <t xml:space="preserve">C00024</t>
@@ -8414,7 +8414,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="N13 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8919,7 +8919,7 @@
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11207,7 +11207,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11378,7 +11378,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11646,7 +11646,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12345,7 +12345,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12531,7 +12531,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12709,7 +12709,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12947,7 +12947,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13647,7 +13647,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13803,7 +13803,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14108,7 +14108,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15306,7 +15306,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15947,7 +15947,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16506,7 +16506,7 @@
   <dimension ref="A1:O95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="topLeft" activeCell="A95" activeCellId="1" sqref="N13 A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19662,7 +19662,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
+      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20146,7 +20146,7 @@
         <v>C00019 - Reduce effect of division-enablers</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="38.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="113.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="s">
         <v>773</v>
       </c>
@@ -20172,8 +20172,8 @@
         <v>726</v>
       </c>
       <c r="M13" s="20"/>
-      <c r="N13" s="52" t="s">
-        <v>416</v>
+      <c r="N13" s="60" t="s">
+        <v>775</v>
       </c>
       <c r="O13" s="24" t="str">
         <f aca="false">A13&amp;" - "&amp;B13</f>
@@ -20182,16 +20182,16 @@
     </row>
     <row r="14" customFormat="false" ht="117.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="24" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>730</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -20209,7 +20209,7 @@
       </c>
       <c r="M14" s="20"/>
       <c r="N14" s="60" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="O14" s="24" t="str">
         <f aca="false">A14&amp;" - "&amp;B14</f>
@@ -20245,7 +20245,7 @@
       </c>
       <c r="M15" s="20"/>
       <c r="N15" s="60" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="O15" s="24" t="str">
         <f aca="false">A15&amp;" - "&amp;B15</f>
@@ -24929,7 +24929,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00019
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2749,9 +2749,17 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">TA08 - Pump Priming
-TA09 - Exposure
-TA10 - Go Physical</t>
+    <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
+T0002 - Facilitate State Propaganda
+T0003 - Leverage Existing Narratives
+T0027 - Adapt existing narratives
+T0028 - Create competing narratives
+T0022 - Conspiracy narratives
+T0023 - Distort facts
+T0053 - Twitter trolls amplify and manipulate
+T0044 - Seed distortions
+T0052 - Teriary sites amplify news
+T0056 - Dedicated channel disseminate information pollution</t>
   </si>
   <si>
     <t xml:space="preserve">C00021</t>
@@ -8414,7 +8422,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="N13 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8919,7 +8927,7 @@
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11207,7 +11215,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11378,7 +11386,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11646,7 +11654,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12345,7 +12353,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12531,7 +12539,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12709,7 +12717,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12947,7 +12955,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13647,7 +13655,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13803,7 +13811,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14108,7 +14116,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15306,7 +15314,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15947,7 +15955,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16506,7 +16514,7 @@
   <dimension ref="A1:O95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="1" sqref="N13 A95"/>
+      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19661,8 +19669,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20138,7 +20146,7 @@
         <v>668</v>
       </c>
       <c r="M12" s="20"/>
-      <c r="N12" s="55" t="s">
+      <c r="N12" s="60" t="s">
         <v>772</v>
       </c>
       <c r="O12" s="24" t="str">
@@ -24929,7 +24937,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00012
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2622,11 +2622,9 @@
     <t xml:space="preserve">2019-11-workshop, 2019-11-search</t>
   </si>
   <si>
-    <t xml:space="preserve">TA07 - Channel Selection
-TA09 - Exposure
-TA10 - Go Physical
-T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
+    <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
 T0002 - Facilitate State Propaganda
+T0003 - Leverage Existing Narratives
 T0007 - Create fake Social Media Profiles / Pages / Groups
 T0008 - Create fake or imposter news sites
 T0009 - Create fake experts
@@ -2647,6 +2645,7 @@
 T0047 - Muzzle social media as a political force
 T0048 - Cow online opinion leaders
 T0049 - Flooding
+T0050 - Cheerleading domestic social media ops
 T0051 - Fabricate social media comment
 T0052 - Tertiary sites amplify news
 T0053 - Twitter trolls amplify and manipulate
@@ -2654,8 +2653,7 @@
 T0055 - Use hashtag
 T0056 - Dedicated channels disseminate information pollution
 T0057 - Organise remote rallies and events
-T0061 - Sell merchandising
-</t>
+T0061 - Sell merchandising</t>
   </si>
   <si>
     <t xml:space="preserve">C00013</t>
@@ -3237,7 +3235,7 @@
 T0052 - Teriary sites amplify news
 T0053 - Twitter trolls amplify and manipulate
 T0054 - Twitter bots amplify
-T0056 – Dedicated channel disseminate information pollution
+T0056 - Dedicated channel disseminate information pollution
 T0057 - Organise remote rallies and events
 T0060 - Continue to amplify
 T0061 - Sell merchandising</t>
@@ -3523,7 +3521,7 @@
     <t xml:space="preserve">C00072</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove non-relevant content from special interest groups – not recommended</t>
+    <t xml:space="preserve">Remove non-relevant content from special interest groups - not recommended</t>
   </si>
   <si>
     <r>
@@ -4561,7 +4559,7 @@
   </si>
   <si>
     <t xml:space="preserve">TA08 - Pump Priming
-TA09 – Exposure
+TA09 - Exposure
 T0053 - Twitter trolls amplify and manipulate
 T0063 - Social media engagement</t>
   </si>
@@ -4914,7 +4912,7 @@
   </si>
   <si>
     <t xml:space="preserve">T0014 - Create funding campaign
-T0017 – Promote online funding</t>
+T0017 - Promote online funding</t>
   </si>
   <si>
     <t xml:space="preserve">C00156</t>
@@ -19774,8 +19772,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20845,7 +20843,7 @@
         <v>726</v>
       </c>
       <c r="M28" s="20"/>
-      <c r="N28" s="60" t="s">
+      <c r="N28" s="56" t="s">
         <v>846</v>
       </c>
       <c r="O28" s="24" t="str">
@@ -21426,7 +21424,7 @@
       </c>
       <c r="O44" s="24" t="str">
         <f aca="false">A44&amp;" - "&amp;B44</f>
-        <v>C00072 - Remove non-relevant content from special interest groups – not recommended</v>
+        <v>C00072 - Remove non-relevant content from special interest groups - not recommended</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="268.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
chg: update countermeasures C00011
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2593,12 +2593,23 @@
     <t xml:space="preserve">A006 - educator,A026 - games designer,A024 - developer</t>
   </si>
   <si>
-    <t xml:space="preserve">TA03 - Develop People
-TA04 - Develop Networks
-TA05 - Microtargeting
-TA08 - Pump Priming
-TA09 - Exposure
-T0059 - Play the long game</t>
+    <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
+T0002 - Facilitate State Propaganda
+T0003 - Leverage Existing Narratives
+T0027 - Adapt existing narratives
+T0028 - Create competing narratives
+T0006 - Create Master Narratives
+T0009 - Create fake experts
+T0008 - Create fake or imposter news sites
+T0013 - Create fake websites
+T0021 - Memes 
+T0025 - Leak altered documents
+T0024 - Create fake videos and images
+T0026 - Create fake research
+T0056 - Dedicated channels disseminate information pollution
+T0051 - Fabricate social media comment
+T0044 - Seed distortions
+T0045 - Use fake experts</t>
   </si>
   <si>
     <t xml:space="preserve">C00012</t>
@@ -7956,16 +7967,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -8389,15 +8400,15 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -19772,8 +19783,8 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20021,7 +20032,7 @@
         <v>712</v>
       </c>
       <c r="M6" s="20"/>
-      <c r="N6" s="55" t="s">
+      <c r="N6" s="59" t="s">
         <v>742</v>
       </c>
       <c r="O6" s="24" t="str">
@@ -20052,7 +20063,7 @@
       <c r="H7" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="60" t="s">
         <v>46</v>
       </c>
       <c r="J7" s="4"/>
@@ -20099,7 +20110,7 @@
         <v>712</v>
       </c>
       <c r="M8" s="20"/>
-      <c r="N8" s="60" t="s">
+      <c r="N8" s="61" t="s">
         <v>754</v>
       </c>
       <c r="O8" s="24" t="str">
@@ -20137,7 +20148,7 @@
         <v>726</v>
       </c>
       <c r="M9" s="20"/>
-      <c r="N9" s="60" t="s">
+      <c r="N9" s="61" t="s">
         <v>759</v>
       </c>
       <c r="O9" s="24" t="str">
@@ -20177,7 +20188,7 @@
         <v>712</v>
       </c>
       <c r="M10" s="20"/>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="61" t="s">
         <v>765</v>
       </c>
       <c r="O10" s="24" t="str">
@@ -20215,7 +20226,7 @@
         <v>668</v>
       </c>
       <c r="M11" s="20"/>
-      <c r="N11" s="60" t="s">
+      <c r="N11" s="61" t="s">
         <v>771</v>
       </c>
       <c r="O11" s="24" t="str">
@@ -20253,7 +20264,7 @@
         <v>668</v>
       </c>
       <c r="M12" s="20"/>
-      <c r="N12" s="61" t="s">
+      <c r="N12" s="59" t="s">
         <v>776</v>
       </c>
       <c r="O12" s="24" t="str">
@@ -20287,7 +20298,7 @@
         <v>726</v>
       </c>
       <c r="M13" s="20"/>
-      <c r="N13" s="61" t="s">
+      <c r="N13" s="59" t="s">
         <v>779</v>
       </c>
       <c r="O13" s="24" t="str">
@@ -20323,7 +20334,7 @@
         <v>726</v>
       </c>
       <c r="M14" s="20"/>
-      <c r="N14" s="61" t="s">
+      <c r="N14" s="59" t="s">
         <v>779</v>
       </c>
       <c r="O14" s="24" t="str">
@@ -20359,7 +20370,7 @@
         <v>726</v>
       </c>
       <c r="M15" s="20"/>
-      <c r="N15" s="61" t="s">
+      <c r="N15" s="59" t="s">
         <v>779</v>
       </c>
       <c r="O15" s="24" t="str">
@@ -20386,7 +20397,7 @@
       <c r="H16" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="I16" s="60" t="s">
         <v>46</v>
       </c>
       <c r="J16" s="4"/>
@@ -20397,7 +20408,7 @@
         <v>726</v>
       </c>
       <c r="M16" s="20"/>
-      <c r="N16" s="61" t="s">
+      <c r="N16" s="59" t="s">
         <v>789</v>
       </c>
       <c r="O16" s="24" t="str">
@@ -20435,7 +20446,7 @@
         <v>794</v>
       </c>
       <c r="M17" s="20"/>
-      <c r="N17" s="61" t="s">
+      <c r="N17" s="59" t="s">
         <v>795</v>
       </c>
       <c r="O17" s="24" t="str">
@@ -20507,7 +20518,7 @@
         <v>668</v>
       </c>
       <c r="M19" s="20"/>
-      <c r="N19" s="60" t="s">
+      <c r="N19" s="61" t="s">
         <v>805</v>
       </c>
       <c r="O19" s="24" t="str">
@@ -20543,7 +20554,7 @@
         <v>668</v>
       </c>
       <c r="M20" s="20"/>
-      <c r="N20" s="60" t="s">
+      <c r="N20" s="61" t="s">
         <v>805</v>
       </c>
       <c r="O20" s="24" t="str">
@@ -20657,7 +20668,7 @@
         <v>726</v>
       </c>
       <c r="M23" s="20"/>
-      <c r="N23" s="60" t="s">
+      <c r="N23" s="61" t="s">
         <v>824</v>
       </c>
       <c r="O23" s="24" t="str">
@@ -20917,7 +20928,7 @@
         <v>794</v>
       </c>
       <c r="M30" s="20"/>
-      <c r="N30" s="61" t="s">
+      <c r="N30" s="59" t="s">
         <v>856</v>
       </c>
       <c r="O30" s="24" t="str">
@@ -20955,7 +20966,7 @@
         <v>712</v>
       </c>
       <c r="M31" s="20"/>
-      <c r="N31" s="61" t="s">
+      <c r="N31" s="59" t="s">
         <v>861</v>
       </c>
       <c r="O31" s="24" t="str">
@@ -21137,7 +21148,7 @@
         <v>712</v>
       </c>
       <c r="M36" s="20"/>
-      <c r="N36" s="60" t="s">
+      <c r="N36" s="61" t="s">
         <v>884</v>
       </c>
       <c r="O36" s="24" t="str">
@@ -21448,7 +21459,7 @@
       <c r="H45" s="24" t="s">
         <v>872</v>
       </c>
-      <c r="I45" s="59" t="s">
+      <c r="I45" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J45" s="4"/>
@@ -23654,7 +23665,7 @@
       <c r="H106" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I106" s="59" t="s">
+      <c r="I106" s="60" t="s">
         <v>49</v>
       </c>
       <c r="J106" s="20"/>
@@ -23770,7 +23781,7 @@
       <c r="H109" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I109" s="59" t="s">
+      <c r="I109" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J109" s="20"/>
@@ -23808,7 +23819,7 @@
       <c r="H110" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I110" s="59" t="s">
+      <c r="I110" s="60" t="s">
         <v>46</v>
       </c>
       <c r="J110" s="20"/>
@@ -23846,7 +23857,7 @@
       <c r="H111" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I111" s="59" t="s">
+      <c r="I111" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J111" s="20"/>
@@ -23884,7 +23895,7 @@
       <c r="H112" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I112" s="59" t="s">
+      <c r="I112" s="60" t="s">
         <v>49</v>
       </c>
       <c r="J112" s="20"/>
@@ -23922,7 +23933,7 @@
       <c r="H113" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I113" s="59" t="s">
+      <c r="I113" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J113" s="20"/>
@@ -23960,7 +23971,7 @@
       <c r="H114" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I114" s="59" t="s">
+      <c r="I114" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J114" s="20"/>
@@ -24036,7 +24047,7 @@
       <c r="H116" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I116" s="59" t="s">
+      <c r="I116" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J116" s="20"/>
@@ -24074,7 +24085,7 @@
       <c r="H117" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I117" s="59" t="s">
+      <c r="I117" s="60" t="s">
         <v>49</v>
       </c>
       <c r="J117" s="20"/>
@@ -24154,7 +24165,7 @@
       <c r="H119" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="I119" s="59" t="s">
+      <c r="I119" s="60" t="s">
         <v>1199</v>
       </c>
       <c r="J119" s="20"/>
@@ -24192,7 +24203,7 @@
       <c r="H120" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I120" s="59" t="s">
+      <c r="I120" s="60" t="s">
         <v>49</v>
       </c>
       <c r="J120" s="20"/>
@@ -24230,7 +24241,7 @@
       <c r="H121" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="I121" s="59" t="s">
+      <c r="I121" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J121" s="20"/>
@@ -24270,7 +24281,7 @@
       <c r="H122" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I122" s="59" t="s">
+      <c r="I122" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J122" s="20"/>
@@ -24348,7 +24359,7 @@
       <c r="H124" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I124" s="59" t="s">
+      <c r="I124" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J124" s="20"/>
@@ -24386,7 +24397,7 @@
       <c r="H125" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I125" s="59" t="s">
+      <c r="I125" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J125" s="20"/>
@@ -24426,7 +24437,7 @@
       <c r="H126" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I126" s="59" t="s">
+      <c r="I126" s="60" t="s">
         <v>1232</v>
       </c>
       <c r="J126" s="20"/>
@@ -24466,7 +24477,7 @@
       <c r="H127" s="24" t="s">
         <v>749</v>
       </c>
-      <c r="I127" s="59" t="s">
+      <c r="I127" s="60" t="s">
         <v>624</v>
       </c>
       <c r="J127" s="20"/>
@@ -24666,7 +24677,7 @@
       <c r="H132" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I132" s="59" t="s">
+      <c r="I132" s="60" t="s">
         <v>46</v>
       </c>
       <c r="J132" s="20"/>
@@ -24782,7 +24793,7 @@
       <c r="H135" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="I135" s="59" t="s">
+      <c r="I135" s="60" t="s">
         <v>46</v>
       </c>
       <c r="J135" s="20"/>

</xml_diff>

<commit_message>
chg: update countermeasures C00010
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2575,8 +2575,8 @@
     <t xml:space="preserve">A020 - policy maker</t>
   </si>
   <si>
-    <t xml:space="preserve">TA05 - Microtargeting
-T00018 - Paid targeted ads</t>
+    <t xml:space="preserve">T0005 - Center of gravity analysis
+T0018 - Paid targeted ads</t>
   </si>
   <si>
     <t xml:space="preserve">C00011</t>
@@ -19783,7 +19783,7 @@
   </sheetPr>
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chg: update countermeasures C00009
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2558,9 +2558,31 @@
     <t xml:space="preserve">A016 - influencer,A006 - educator</t>
   </si>
   <si>
-    <t xml:space="preserve">TA08 - Pump Priming
-T0010 - Cultivate ignorant agents
-T0029 - Manipulate online polls</t>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">T0010 - Cultivate ignorant agents
+T0039 - Bait legitimate influencers
+T0044 - Seed distortions
+T0042 - Kernel of truth
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">T0048 - Cow online opinion leaders
+T0052 - Tertiary sites amplify news
+T0053 - Twitter trolls amplify and manipulate
+T0055 - Use hashtag
+T0056 - Dedicated channels disseminate information pollution</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">C00010</t>
@@ -19784,7 +19806,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19928,7 +19950,7 @@
         <v>C00008 - Create shared fact-checking database</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="52.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
         <v>728</v>
       </c>

</xml_diff>

<commit_message>
chg: update countermeasures C00008
</commit_message>
<xml_diff>
--- a/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
+++ b/AMITT_MASTER_DATA/AMITT_TTPs_MASTER.xlsx
@@ -2536,14 +2536,24 @@
     <t xml:space="preserve">D4 Degrade</t>
   </si>
   <si>
-    <t xml:space="preserve">TA01 - Strategic Planning
-TA06 - Develop Content
-TA08 - Pump Priming
+    <t xml:space="preserve">T0001 - 5Ds (dismiss, distort, distract, dismay, divide)
+T0002 - Facilitate State Propaganda
+T0003 - Leverage Existing Narratives
+T0027 - Adapt existing narratives
+T0028 - Create competing narratives
 T0006 - Create Master Narratives
 T0009 - Create fake experts
 T0008 - Create fake or imposter news sites
 T0013 - Create fake websites
-T0014 - Create funding campaigns</t>
+T0014 - Create funding campaigns
+T0021 - Memes 
+T0025 - Leak altered documents
+T0024 - Create fake videos and images
+T0026 - Create fake research
+T0056 - Dedicated channels disseminate information pollution
+T0051 - Fabricate social media comment
+T0044 - Seed distortions
+T0045 - Use fake experts</t>
   </si>
   <si>
     <t xml:space="preserve">C00009</t>
@@ -19806,7 +19816,7 @@
   <dimension ref="A1:O142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19942,7 +19952,7 @@
         <v>726</v>
       </c>
       <c r="M3" s="20"/>
-      <c r="N3" s="55" t="s">
+      <c r="N3" s="59" t="s">
         <v>727</v>
       </c>
       <c r="O3" s="24" t="str">

</xml_diff>